<commit_message>
Fixed the minus in third derivate relation
</commit_message>
<xml_diff>
--- a/Project/IAG Solar Flux Atlas/Infrared range/Data/valores_NIR.xlsx
+++ b/Project/IAG Solar Flux Atlas/Infrared range/Data/valores_NIR.xlsx
@@ -438,7 +438,7 @@
         <v>1092414854.350568</v>
       </c>
       <c r="F2">
-        <v>-1.544647344879015E-08</v>
+        <v>-156677110.1056063</v>
       </c>
       <c r="G2">
         <v>209.110092138397</v>
@@ -461,7 +461,7 @@
         <v>5206248583.586316</v>
       </c>
       <c r="F3">
-        <v>1.802524638120297E-09</v>
+        <v>18519209.4692356</v>
       </c>
       <c r="G3">
         <v>363.2835654082753</v>
@@ -484,7 +484,7 @@
         <v>1039916995.203525</v>
       </c>
       <c r="F4">
-        <v>-9.262597084721621E-09</v>
+        <v>-95784039.45845836</v>
       </c>
       <c r="G4">
         <v>300.2634136864436</v>
@@ -507,7 +507,7 @@
         <v>680676876.5583919</v>
       </c>
       <c r="F5">
-        <v>-2.270660566395253E-08</v>
+        <v>-235150854.3567928</v>
       </c>
       <c r="G5">
         <v>249.632867166849</v>
@@ -530,7 +530,7 @@
         <v>579920772.9419634</v>
       </c>
       <c r="F6">
-        <v>2.07786550985991E-08</v>
+        <v>215585189.2373232</v>
       </c>
       <c r="G6">
         <v>-118.817428870391</v>
@@ -553,7 +553,7 @@
         <v>2487722571.704799</v>
       </c>
       <c r="F7">
-        <v>-5.983817182501139E-09</v>
+        <v>-62683098.96488434</v>
       </c>
       <c r="G7">
         <v>231.1386673049972</v>
@@ -576,7 +576,7 @@
         <v>1164347933.249144</v>
       </c>
       <c r="F8">
-        <v>-1.576064356964532E-08</v>
+        <v>-166611754.3473985</v>
       </c>
       <c r="G8">
         <v>53.21822221639219</v>
@@ -599,7 +599,7 @@
         <v>1427904249.565825</v>
       </c>
       <c r="F9">
-        <v>2.138956934231155E-09</v>
+        <v>22663026.0553909</v>
       </c>
       <c r="G9">
         <v>132.9702376056558</v>
@@ -622,7 +622,7 @@
         <v>4861451483.351841</v>
       </c>
       <c r="F10">
-        <v>2.678436347988159E-09</v>
+        <v>28409543.72762407</v>
       </c>
       <c r="G10">
         <v>369.2627661837664</v>
@@ -645,7 +645,7 @@
         <v>2369787863.916452</v>
       </c>
       <c r="F11">
-        <v>-4.266898279241372E-09</v>
+        <v>-45429471.48641107</v>
       </c>
       <c r="G11">
         <v>221.3481712655098</v>
@@ -668,7 +668,7 @@
         <v>2893465557.268535</v>
       </c>
       <c r="F12">
-        <v>-4.887100847058805E-09</v>
+        <v>-52285354.05180201</v>
       </c>
       <c r="G12">
         <v>203.3938889715005</v>
@@ -691,7 +691,7 @@
         <v>4898282972.106872</v>
       </c>
       <c r="F13">
-        <v>6.694145581171454E-10</v>
+        <v>7300468.186603961</v>
       </c>
       <c r="G13">
         <v>440.04664022485</v>
@@ -714,7 +714,7 @@
         <v>4769684636.022537</v>
       </c>
       <c r="F14">
-        <v>-3.466232884930975E-10</v>
+        <v>-3783279.059394291</v>
       </c>
       <c r="G14">
         <v>196.5138348174656</v>
@@ -737,7 +737,7 @@
         <v>1175894603.604178</v>
       </c>
       <c r="F15">
-        <v>-9.144346224379187E-09</v>
+        <v>-101648915.6019635</v>
       </c>
       <c r="G15">
         <v>163.5013882968728</v>
@@ -760,7 +760,7 @@
         <v>517253609.0199448</v>
       </c>
       <c r="F16">
-        <v>3.198266206485156E-09</v>
+        <v>35809794.85313801</v>
       </c>
       <c r="G16">
         <v>58.2879763077196</v>
@@ -783,7 +783,7 @@
         <v>651237286.9919277</v>
       </c>
       <c r="F17">
-        <v>-3.594523913798455E-08</v>
+        <v>-406184614.3090176</v>
       </c>
       <c r="G17">
         <v>55.24638439732712</v>
@@ -806,7 +806,7 @@
         <v>1483377073.555127</v>
       </c>
       <c r="F18">
-        <v>-7.712425790168475E-09</v>
+        <v>-87995685.52016665</v>
       </c>
       <c r="G18">
         <v>240.7584556362024</v>
@@ -829,7 +829,7 @@
         <v>5741618897.409628</v>
       </c>
       <c r="F19">
-        <v>-2.910778773170599E-10</v>
+        <v>-3332097.627462617</v>
       </c>
       <c r="G19">
         <v>234.7626117048913</v>
@@ -852,7 +852,7 @@
         <v>816452194.0869088</v>
       </c>
       <c r="F20">
-        <v>-2.109449834150542E-09</v>
+        <v>-24187923.80759507</v>
       </c>
       <c r="G20">
         <v>78.22169691553601</v>
@@ -875,7 +875,7 @@
         <v>3023016423.668905</v>
       </c>
       <c r="F21">
-        <v>-8.514947215188506E-11</v>
+        <v>-977415.4649770735</v>
       </c>
       <c r="G21">
         <v>211.4314352049752</v>
@@ -898,7 +898,7 @@
         <v>2268074095.879919</v>
       </c>
       <c r="F22">
-        <v>-4.452903509609485E-09</v>
+        <v>-51229562.94007045</v>
       </c>
       <c r="G22">
         <v>188.1546650230045</v>
@@ -921,7 +921,7 @@
         <v>1167710602.469932</v>
       </c>
       <c r="F23">
-        <v>-8.771544740724401E-09</v>
+        <v>-101261740.0364153</v>
       </c>
       <c r="G23">
         <v>156.1789013206684</v>
@@ -944,7 +944,7 @@
         <v>2620537720.623078</v>
       </c>
       <c r="F24">
-        <v>-7.416718898480453E-10</v>
+        <v>-8616107.045082089</v>
       </c>
       <c r="G24">
         <v>150.158336158803</v>
@@ -967,7 +967,7 @@
         <v>912103665.3756156</v>
       </c>
       <c r="F25">
-        <v>-1.332371307494179E-08</v>
+        <v>-155365542.5129987</v>
       </c>
       <c r="G25">
         <v>201.9466609972183</v>
@@ -990,7 +990,7 @@
         <v>6334397162.849628</v>
       </c>
       <c r="F26">
-        <v>4.805954238448229E-10</v>
+        <v>5619379.032977202</v>
       </c>
       <c r="G26">
         <v>242.1715747933119</v>
@@ -1013,7 +1013,7 @@
         <v>2907342842.092541</v>
       </c>
       <c r="F27">
-        <v>-1.988145627639873E-09</v>
+        <v>-23491007.64812877</v>
       </c>
       <c r="G27">
         <v>238.6633748817404</v>
@@ -1036,7 +1036,7 @@
         <v>3650308171.970758</v>
       </c>
       <c r="F28">
-        <v>4.113384981737244E-10</v>
+        <v>4861517.001753004</v>
       </c>
       <c r="G28">
         <v>209.894352961243</v>
@@ -1059,7 +1059,7 @@
         <v>5367784831.088258</v>
       </c>
       <c r="F29">
-        <v>6.074186494679827E-10</v>
+        <v>7306275.050283175</v>
       </c>
       <c r="G29">
         <v>437.9865704075818</v>
@@ -1082,7 +1082,7 @@
         <v>5502191211.121552</v>
       </c>
       <c r="F30">
-        <v>-2.977058105338346E-10</v>
+        <v>-3667309.38911736</v>
       </c>
       <c r="G30">
         <v>338.6320776117072</v>
@@ -1105,7 +1105,7 @@
         <v>1109103792.656712</v>
       </c>
       <c r="F31">
-        <v>-2.019763207059904E-09</v>
+        <v>-25102531.12714076</v>
       </c>
       <c r="G31">
         <v>164.6814456252225</v>
@@ -1128,7 +1128,7 @@
         <v>2276211567.059862</v>
       </c>
       <c r="F32">
-        <v>-1.91495584472234E-09</v>
+        <v>-23994375.32402267</v>
       </c>
       <c r="G32">
         <v>277.6895329283418</v>
@@ -1151,7 +1151,7 @@
         <v>2230216978.745636</v>
       </c>
       <c r="F33">
-        <v>-2.222223980356118E-09</v>
+        <v>-28263552.39839941</v>
       </c>
       <c r="G33">
         <v>175.0261407137777</v>
@@ -1174,7 +1174,7 @@
         <v>4012371034.929343</v>
       </c>
       <c r="F34">
-        <v>-7.439869638292425E-10</v>
+        <v>-9957776.974086111</v>
       </c>
       <c r="G34">
         <v>253.6373431923298</v>
@@ -1197,7 +1197,7 @@
         <v>1423530335.532048</v>
       </c>
       <c r="F35">
-        <v>-3.574845553543127E-09</v>
+        <v>-48341681.80190385</v>
       </c>
       <c r="G35">
         <v>294.6869318163317</v>
@@ -1220,7 +1220,7 @@
         <v>5131435504.372919</v>
       </c>
       <c r="F36">
-        <v>-6.234912603522473E-10</v>
+        <v>-8438671.782919452</v>
       </c>
       <c r="G36">
         <v>208.4593297016262</v>
@@ -1243,7 +1243,7 @@
         <v>3567627233.572556</v>
       </c>
       <c r="F37">
-        <v>-9.984103487400643E-10</v>
+        <v>-13690480.77423065</v>
       </c>
       <c r="G37">
         <v>257.6479066640685</v>
@@ -1266,7 +1266,7 @@
         <v>3740177205.343518</v>
       </c>
       <c r="F38">
-        <v>-4.044165556128844E-10</v>
+        <v>-5682019.626809872</v>
       </c>
       <c r="G38">
         <v>278.1147539102653</v>
@@ -1289,7 +1289,7 @@
         <v>4551789703.786042</v>
       </c>
       <c r="F39">
-        <v>5.224970366534061E-10</v>
+        <v>7373565.200082134</v>
       </c>
       <c r="G39">
         <v>228.2972618982217</v>
@@ -1312,7 +1312,7 @@
         <v>3735533218.436416</v>
       </c>
       <c r="F40">
-        <v>-3.947218141290915E-09</v>
+        <v>-58420175.82534759</v>
       </c>
       <c r="G40">
         <v>-78.82258140793543</v>
@@ -1335,7 +1335,7 @@
         <v>5920332872.86448</v>
       </c>
       <c r="F41">
-        <v>5.450860916911807E-10</v>
+        <v>8343150.216613088</v>
       </c>
       <c r="G41">
         <v>293.786195995636</v>
@@ -1358,7 +1358,7 @@
         <v>1719662461.027918</v>
       </c>
       <c r="F42">
-        <v>1.058086426772724E-09</v>
+        <v>17818425.38171053</v>
       </c>
       <c r="G42">
         <v>60.52873280376289</v>
@@ -1381,7 +1381,7 @@
         <v>2052153873.602626</v>
       </c>
       <c r="F43">
-        <v>-3.620125573484368E-10</v>
+        <v>-6126794.508152236</v>
       </c>
       <c r="G43">
         <v>84.10917700767887</v>
@@ -1404,7 +1404,7 @@
         <v>5053048059.109766</v>
       </c>
       <c r="F44">
-        <v>-1.600231929229753E-09</v>
+        <v>-29709112.09872661</v>
       </c>
       <c r="G44">
         <v>195.1901477600028</v>
@@ -1427,7 +1427,7 @@
         <v>4078361117.601238</v>
       </c>
       <c r="F45">
-        <v>1.662864922461764E-09</v>
+        <v>33204587.71600025</v>
       </c>
       <c r="G45">
         <v>448.9066877308219</v>
@@ -1450,7 +1450,7 @@
         <v>3234104353.83377</v>
       </c>
       <c r="F46">
-        <v>3.979092676984455E-10</v>
+        <v>7962682.93565054</v>
       </c>
       <c r="G46">
         <v>161.3177175190825</v>
@@ -1473,7 +1473,7 @@
         <v>3292310950.058791</v>
       </c>
       <c r="F47">
-        <v>3.939135022071648E-10</v>
+        <v>8322813.517383904</v>
       </c>
       <c r="G47">
         <v>213.8464966395116</v>
@@ -1496,7 +1496,7 @@
         <v>484919102.1449975</v>
       </c>
       <c r="F48">
-        <v>1.736915421216534E-09</v>
+        <v>37658692.86906283</v>
       </c>
       <c r="G48">
         <v>-51.88218762412625</v>
@@ -1519,7 +1519,7 @@
         <v>1956128998.876171</v>
       </c>
       <c r="F49">
-        <v>-2.833159523882541E-09</v>
+        <v>-63107876.30689377</v>
       </c>
       <c r="G49">
         <v>68.71090987194373</v>
@@ -1542,7 +1542,7 @@
         <v>3958370237.736347</v>
       </c>
       <c r="F50">
-        <v>-3.3348344075996E-10</v>
+        <v>-7461850.332053294</v>
       </c>
       <c r="G50">
         <v>213.2540066162134</v>
@@ -1565,7 +1565,7 @@
         <v>885320110.7129227</v>
       </c>
       <c r="F51">
-        <v>7.929103294786978E-10</v>
+        <v>18408945.50113069</v>
       </c>
       <c r="G51">
         <v>55.85954716125617</v>
@@ -1588,7 +1588,7 @@
         <v>2893479150.314776</v>
       </c>
       <c r="F52">
-        <v>-1.111899631608442E-09</v>
+        <v>-25835291.56025861</v>
       </c>
       <c r="G52">
         <v>281.6710125485241</v>
@@ -1611,7 +1611,7 @@
         <v>856868878.490669</v>
       </c>
       <c r="F53">
-        <v>-5.173699641342938E-09</v>
+        <v>-126876111.3540012</v>
       </c>
       <c r="G53">
         <v>359.3501419186555</v>
@@ -1634,7 +1634,7 @@
         <v>3698188201.947296</v>
       </c>
       <c r="F54">
-        <v>-2.871944168954919E-10</v>
+        <v>-7148187.431506136</v>
       </c>
       <c r="G54">
         <v>221.9724054358576</v>
@@ -1657,7 +1657,7 @@
         <v>2922384018.712894</v>
       </c>
       <c r="F55">
-        <v>3.489170536384955E-10</v>
+        <v>8848614.204445509</v>
       </c>
       <c r="G55">
         <v>225.6869093191555</v>
@@ -1680,7 +1680,7 @@
         <v>4279152310.849101</v>
       </c>
       <c r="F56">
-        <v>1.60953830371774E-10</v>
+        <v>4111393.746382472</v>
       </c>
       <c r="G56">
         <v>350.9627206966982</v>
@@ -1703,7 +1703,7 @@
         <v>2966110426.167465</v>
       </c>
       <c r="F57">
-        <v>2.678671249737209E-09</v>
+        <v>68640944.86805318</v>
       </c>
       <c r="G57">
         <v>-127.9523652009337</v>
@@ -1726,7 +1726,7 @@
         <v>3337081972.08334</v>
       </c>
       <c r="F58">
-        <v>-4.752497212969687E-10</v>
+        <v>-12799969.90510492</v>
       </c>
       <c r="G58">
         <v>334.645859331857</v>
@@ -1749,7 +1749,7 @@
         <v>2273626482.28181</v>
       </c>
       <c r="F59">
-        <v>-1.514495446272845E-10</v>
+        <v>-4101617.602997416</v>
       </c>
       <c r="G59">
         <v>236.03185496702</v>
@@ -1772,7 +1772,7 @@
         <v>1663237571.869143</v>
       </c>
       <c r="F60">
-        <v>-9.000757677092382E-10</v>
+        <v>-24495923.06465667</v>
       </c>
       <c r="G60">
         <v>315.1020603992357</v>
@@ -1795,7 +1795,7 @@
         <v>5652830475.671362</v>
       </c>
       <c r="F61">
-        <v>2.362065338414572E-11</v>
+        <v>650730.1445753785</v>
       </c>
       <c r="G61">
         <v>269.930418796854</v>
@@ -1818,7 +1818,7 @@
         <v>1054536340.142622</v>
       </c>
       <c r="F62">
-        <v>-7.711335573937575E-09</v>
+        <v>-215975076.2760331</v>
       </c>
       <c r="G62">
         <v>171.488168777924</v>
@@ -1841,7 +1841,7 @@
         <v>3940752423.939021</v>
       </c>
       <c r="F63">
-        <v>5.386407248620398E-10</v>
+        <v>17138920.22262292</v>
       </c>
       <c r="G63">
         <v>170.5938907839318</v>
@@ -1864,7 +1864,7 @@
         <v>3645317858.151546</v>
       </c>
       <c r="F64">
-        <v>8.60295996629768E-10</v>
+        <v>27702535.8647331</v>
       </c>
       <c r="G64">
         <v>273.0316685858902</v>
@@ -1887,7 +1887,7 @@
         <v>4176362792.286147</v>
       </c>
       <c r="F65">
-        <v>-2.490967281152965E-10</v>
+        <v>-11991303.16024815</v>
       </c>
       <c r="G65">
         <v>-22.26326037205379</v>
@@ -1910,7 +1910,7 @@
         <v>2510051758.391216</v>
       </c>
       <c r="F66">
-        <v>4.77796251830911E-10</v>
+        <v>23559156.52719074</v>
       </c>
       <c r="G66">
         <v>-142.8399188742064</v>
@@ -1933,7 +1933,7 @@
         <v>3416335965.676072</v>
       </c>
       <c r="F67">
-        <v>8.435027721677635E-11</v>
+        <v>4225147.812217094</v>
       </c>
       <c r="G67">
         <v>210.4124623500545</v>
@@ -1956,7 +1956,7 @@
         <v>5251662869.876287</v>
       </c>
       <c r="F68">
-        <v>1.127908335814722E-09</v>
+        <v>56996246.20949438</v>
       </c>
       <c r="G68">
         <v>43.98963272055954</v>
@@ -1979,7 +1979,7 @@
         <v>2350162102.19848</v>
       </c>
       <c r="F69">
-        <v>-3.619863544521422E-10</v>
+        <v>-18432425.35255145</v>
       </c>
       <c r="G69">
         <v>283.3915436144903</v>
@@ -2002,7 +2002,7 @@
         <v>3532133521.254247</v>
       </c>
       <c r="F70">
-        <v>3.824614616370363E-10</v>
+        <v>19652248.51544683</v>
       </c>
       <c r="G70">
         <v>346.4689432125126</v>
@@ -2025,7 +2025,7 @@
         <v>3476608258.668179</v>
       </c>
       <c r="F71">
-        <v>-3.845809865903759E-11</v>
+        <v>-1998760.828410971</v>
       </c>
       <c r="G71">
         <v>75.45033175572252</v>
@@ -2048,7 +2048,7 @@
         <v>3258857784.176424</v>
       </c>
       <c r="F72">
-        <v>1.772763240092996E-10</v>
+        <v>9281268.46865187</v>
       </c>
       <c r="G72">
         <v>182.3348335479448</v>
@@ -2071,7 +2071,7 @@
         <v>1854800454.515697</v>
       </c>
       <c r="F73">
-        <v>7.358239498076856E-10</v>
+        <v>39080523.23495647</v>
       </c>
       <c r="G73">
         <v>69.11817059749109</v>
@@ -2094,7 +2094,7 @@
         <v>3705141813.06572</v>
       </c>
       <c r="F74">
-        <v>4.342523919774367E-10</v>
+        <v>23251624.81021379</v>
       </c>
       <c r="G74">
         <v>277.8832990826441</v>
@@ -2117,7 +2117,7 @@
         <v>3223982704.849172</v>
       </c>
       <c r="F75">
-        <v>2.774998532271235E-10</v>
+        <v>14905797.98844591</v>
       </c>
       <c r="G75">
         <v>387.9398314054862</v>
@@ -2140,7 +2140,7 @@
         <v>2355292363.132841</v>
       </c>
       <c r="F76">
-        <v>7.454143167504333E-11</v>
+        <v>4009330.396214958</v>
       </c>
       <c r="G76">
         <v>157.4861582376646</v>
@@ -2163,7 +2163,7 @@
         <v>3630380395.531632</v>
       </c>
       <c r="F77">
-        <v>3.333472138739946E-10</v>
+        <v>18025201.92779333</v>
       </c>
       <c r="G77">
         <v>334.2137252694796</v>
@@ -2186,7 +2186,7 @@
         <v>1107639082.173041</v>
       </c>
       <c r="F78">
-        <v>4.817097792729077E-09</v>
+        <v>260580081.1625765</v>
       </c>
       <c r="G78">
         <v>102.2198540424131</v>
@@ -2209,7 +2209,7 @@
         <v>3322326761.809361</v>
       </c>
       <c r="F79">
-        <v>-1.203964150174483E-10</v>
+        <v>-6520566.126871623</v>
       </c>
       <c r="G79">
         <v>485.4007268146134</v>
@@ -2232,7 +2232,7 @@
         <v>674786405.2326441</v>
       </c>
       <c r="F80">
-        <v>-2.111999337624869E-11</v>
+        <v>-1157440.795803524</v>
       </c>
       <c r="G80">
         <v>3.918767101372705</v>
@@ -2255,7 +2255,7 @@
         <v>3256569347.414473</v>
       </c>
       <c r="F81">
-        <v>-3.772373605008784E-10</v>
+        <v>-20886780.63261012</v>
       </c>
       <c r="G81">
         <v>537.452358866126</v>
@@ -2278,7 +2278,7 @@
         <v>2755933012.006021</v>
       </c>
       <c r="F82">
-        <v>7.237259440681476E-10</v>
+        <v>40158856.45263437</v>
       </c>
       <c r="G82">
         <v>101.5716236259524</v>
@@ -2301,7 +2301,7 @@
         <v>1496411122.723968</v>
       </c>
       <c r="F83">
-        <v>-1.778411852507746E-09</v>
+        <v>-102506662.6875892</v>
       </c>
       <c r="G83">
         <v>243.7876290177686</v>
@@ -2324,7 +2324,7 @@
         <v>1369355575.743196</v>
       </c>
       <c r="F84">
-        <v>-1.711961314276328E-09</v>
+        <v>-99287991.6351856</v>
       </c>
       <c r="G84">
         <v>251.1387476538749</v>
@@ -2347,7 +2347,7 @@
         <v>1331376628.093632</v>
       </c>
       <c r="F85">
-        <v>-1.024251714651252E-09</v>
+        <v>-59480893.18530277</v>
       </c>
       <c r="G85">
         <v>46.34888772717395</v>
@@ -2370,7 +2370,7 @@
         <v>3060273067.410341</v>
       </c>
       <c r="F86">
-        <v>1.939881035459793E-10</v>
+        <v>11301427.42831764</v>
       </c>
       <c r="G86">
         <v>175.5993074487081</v>
@@ -2393,7 +2393,7 @@
         <v>3785816998.200178</v>
       </c>
       <c r="F87">
-        <v>2.643008629337893E-10</v>
+        <v>15407605.52427121</v>
       </c>
       <c r="G87">
         <v>191.0060096595961</v>
@@ -2416,7 +2416,7 @@
         <v>3349839984.879492</v>
       </c>
       <c r="F88">
-        <v>-1.971909422738155E-10</v>
+        <v>-11518568.90202348</v>
       </c>
       <c r="G88">
         <v>-7.713523254235525</v>
@@ -2439,7 +2439,7 @@
         <v>2115502168.66674</v>
       </c>
       <c r="F89">
-        <v>3.081673816930199E-10</v>
+        <v>18044504.93170052</v>
       </c>
       <c r="G89">
         <v>304.5009523394917</v>
@@ -2462,7 +2462,7 @@
         <v>1727811374.925148</v>
       </c>
       <c r="F90">
-        <v>-6.841231640197701E-10</v>
+        <v>-40216141.81642985</v>
       </c>
       <c r="G90">
         <v>336.9323512893235</v>
@@ -2485,7 +2485,7 @@
         <v>3345003900.470722</v>
       </c>
       <c r="F91">
-        <v>-1.263194239692884E-10</v>
+        <v>-7466818.371781709</v>
       </c>
       <c r="G91">
         <v>-34.60802334615429</v>
@@ -2508,7 +2508,7 @@
         <v>1763419783.923234</v>
       </c>
       <c r="F92">
-        <v>-9.645175875375924E-10</v>
+        <v>-57039602.0169448</v>
       </c>
       <c r="G92">
         <v>272.9875613605734</v>
@@ -2531,7 +2531,7 @@
         <v>641019393.6751802</v>
       </c>
       <c r="F93">
-        <v>-2.978040033953045E-09</v>
+        <v>-176514311.1066101</v>
       </c>
       <c r="G93">
         <v>265.147676599972</v>
@@ -2554,7 +2554,7 @@
         <v>2128410984.442255</v>
       </c>
       <c r="F94">
-        <v>4.926582417161018E-10</v>
+        <v>29292744.5491517</v>
       </c>
       <c r="G94">
         <v>247.660755848954</v>
@@ -2577,7 +2577,7 @@
         <v>1920806518.761335</v>
       </c>
       <c r="F95">
-        <v>2.427742705996022E-10</v>
+        <v>14444204.9751977</v>
       </c>
       <c r="G95">
         <v>99.81629483784745</v>
@@ -2600,7 +2600,7 @@
         <v>3308374422.757637</v>
       </c>
       <c r="F96">
-        <v>2.168318768521223E-10</v>
+        <v>12927320.51711405</v>
       </c>
       <c r="G96">
         <v>368.3630993007404</v>
@@ -2623,7 +2623,7 @@
         <v>3708052043.393218</v>
       </c>
       <c r="F97">
-        <v>2.6006551038856E-10</v>
+        <v>15545737.79064793</v>
       </c>
       <c r="G97">
         <v>230.0753746088103</v>
@@ -2646,7 +2646,7 @@
         <v>1337421639.484831</v>
       </c>
       <c r="F98">
-        <v>-2.006706151294938E-10</v>
+        <v>-12035485.47258861</v>
       </c>
       <c r="G98">
         <v>114.9415798028418</v>
@@ -2669,7 +2669,7 @@
         <v>3638577979.461855</v>
       </c>
       <c r="F99">
-        <v>8.878660644056583E-11</v>
+        <v>5329848.285221979</v>
       </c>
       <c r="G99">
         <v>42.13583432360907</v>
@@ -2692,7 +2692,7 @@
         <v>2776986058.737023</v>
       </c>
       <c r="F100">
-        <v>9.191969754054452E-11</v>
+        <v>5524094.789445193</v>
       </c>
       <c r="G100">
         <v>271.8919236143388</v>
@@ -2715,7 +2715,7 @@
         <v>3431266749.599977</v>
       </c>
       <c r="F101">
-        <v>1.020106396373729E-10</v>
+        <v>6144866.720842819</v>
       </c>
       <c r="G101">
         <v>256.424267459517</v>
@@ -2738,7 +2738,7 @@
         <v>2161430199.950818</v>
       </c>
       <c r="F102">
-        <v>6.555600247180679E-10</v>
+        <v>39521753.0038707</v>
       </c>
       <c r="G102">
         <v>53.57015187109182</v>
@@ -2761,7 +2761,7 @@
         <v>2958394824.958137</v>
       </c>
       <c r="F103">
-        <v>-2.15659309188655E-09</v>
+        <v>-130391513.3155631</v>
       </c>
       <c r="G103">
         <v>30.58936425919826</v>
@@ -2784,7 +2784,7 @@
         <v>3358313621.082551</v>
       </c>
       <c r="F104">
-        <v>1.554510683503789E-11</v>
+        <v>940112.4217698813</v>
       </c>
       <c r="G104">
         <v>281.0230382164584</v>
@@ -2807,7 +2807,7 @@
         <v>1497438084.829989</v>
       </c>
       <c r="F105">
-        <v>2.309440548178703E-10</v>
+        <v>13984483.06792466</v>
       </c>
       <c r="G105">
         <v>309.6002183101011</v>
@@ -2830,7 +2830,7 @@
         <v>3691882257.913296</v>
       </c>
       <c r="F106">
-        <v>-1.170116905012646E-09</v>
+        <v>-70925485.27770038</v>
       </c>
       <c r="G106">
         <v>43.94458190379509</v>
@@ -2853,7 +2853,7 @@
         <v>3389258173.328023</v>
       </c>
       <c r="F107">
-        <v>2.164706413129103E-10</v>
+        <v>13139329.48703831</v>
       </c>
       <c r="G107">
         <v>374.3551108861444</v>
@@ -2876,7 +2876,7 @@
         <v>3360735596.695724</v>
       </c>
       <c r="F108">
-        <v>2.327925568053411E-11</v>
+        <v>1424466.953564628</v>
       </c>
       <c r="G108">
         <v>249.7017225159084</v>
@@ -2899,7 +2899,7 @@
         <v>2775194890.509315</v>
       </c>
       <c r="F109">
-        <v>7.437264700678302E-10</v>
+        <v>46096031.02674194</v>
       </c>
       <c r="G109">
         <v>98.80106273223207</v>
@@ -2922,7 +2922,7 @@
         <v>3272568222.625025</v>
       </c>
       <c r="F110">
-        <v>2.019138068125297E-11</v>
+        <v>1256206.585799897</v>
       </c>
       <c r="G110">
         <v>324.5962672596718</v>
@@ -2945,7 +2945,7 @@
         <v>853750483.476817</v>
       </c>
       <c r="F111">
-        <v>3.718008137255712E-10</v>
+        <v>23232924.08383252</v>
       </c>
       <c r="G111">
         <v>-7.584593315247607</v>
@@ -2968,7 +2968,7 @@
         <v>1984738847.859315</v>
       </c>
       <c r="F112">
-        <v>5.389205068134685E-11</v>
+        <v>3376419.004386254</v>
       </c>
       <c r="G112">
         <v>100.4300806716848</v>
@@ -2991,7 +2991,7 @@
         <v>2977581355.170902</v>
       </c>
       <c r="F113">
-        <v>6.703980115782846E-11</v>
+        <v>4201763.757616004</v>
       </c>
       <c r="G113">
         <v>414.9451478422461</v>
@@ -3014,7 +3014,7 @@
         <v>2551710361.498037</v>
       </c>
       <c r="F114">
-        <v>-4.047476472060265E-10</v>
+        <v>-25374146.47156611</v>
       </c>
       <c r="G114">
         <v>208.4068130961335</v>
@@ -3037,7 +3037,7 @@
         <v>2189644938.355878</v>
       </c>
       <c r="F115">
-        <v>-2.859153677706259E-10</v>
+        <v>-17936058.31621805</v>
       </c>
       <c r="G115">
         <v>172.3812270593169</v>
@@ -3060,7 +3060,7 @@
         <v>4022960594.522149</v>
       </c>
       <c r="F116">
-        <v>-2.045033927083868E-10</v>
+        <v>-12832525.2108562</v>
       </c>
       <c r="G116">
         <v>225.4058009455241</v>
@@ -3083,7 +3083,7 @@
         <v>3121919735.65976</v>
       </c>
       <c r="F117">
-        <v>-3.67878130495912E-11</v>
+        <v>-2315641.968682407</v>
       </c>
       <c r="G117">
         <v>431.5333003021923</v>
@@ -3106,7 +3106,7 @@
         <v>1535985471.910607</v>
       </c>
       <c r="F118">
-        <v>1.191231239534638E-09</v>
+        <v>75078379.31545964</v>
       </c>
       <c r="G118">
         <v>361.3889672487713</v>
@@ -3129,7 +3129,7 @@
         <v>1731865508.150192</v>
       </c>
       <c r="F119">
-        <v>1.155247911768087E-09</v>
+        <v>73051761.23565413</v>
       </c>
       <c r="G119">
         <v>1.890522443555685</v>
@@ -3152,7 +3152,7 @@
         <v>3139864006.512664</v>
       </c>
       <c r="F120">
-        <v>4.210474665832931E-10</v>
+        <v>26694836.80401955</v>
       </c>
       <c r="G120">
         <v>360.8531826447532</v>
@@ -3175,7 +3175,7 @@
         <v>972403926.8396584</v>
       </c>
       <c r="F121">
-        <v>-4.559741636731931E-09</v>
+        <v>-289160107.4694867</v>
       </c>
       <c r="G121">
         <v>253.149067868522</v>
@@ -3198,7 +3198,7 @@
         <v>3555038684.349282</v>
       </c>
       <c r="F122">
-        <v>1.793166977247336E-10</v>
+        <v>11382656.53319679</v>
       </c>
       <c r="G122">
         <v>330.5243848898632</v>
@@ -3221,7 +3221,7 @@
         <v>3312740761.39504</v>
       </c>
       <c r="F123">
-        <v>-1.231144987820593E-10</v>
+        <v>-7834604.476762424</v>
       </c>
       <c r="G123">
         <v>166.1026827974451</v>
@@ -3244,7 +3244,7 @@
         <v>1441603979.621701</v>
       </c>
       <c r="F124">
-        <v>1.825050425095563E-09</v>
+        <v>116512923.8326921</v>
       </c>
       <c r="G124">
         <v>248.9546179611329</v>
@@ -3267,7 +3267,7 @@
         <v>3151944383.743469</v>
       </c>
       <c r="F125">
-        <v>-1.188465754803765E-10</v>
+        <v>-7595046.538135923</v>
       </c>
       <c r="G125">
         <v>328.0835720292703</v>
@@ -3290,7 +3290,7 @@
         <v>2723534864.191213</v>
       </c>
       <c r="F126">
-        <v>1.458785483341701E-10</v>
+        <v>9337295.743194398</v>
       </c>
       <c r="G126">
         <v>82.93084284040249</v>
@@ -3313,7 +3313,7 @@
         <v>3508808338.613146</v>
       </c>
       <c r="F127">
-        <v>5.411076339186132E-10</v>
+        <v>34674361.21255974</v>
       </c>
       <c r="G127">
         <v>258.1430529977978</v>
@@ -3336,7 +3336,7 @@
         <v>3318848889.865634</v>
       </c>
       <c r="F128">
-        <v>3.10444611102737E-10</v>
+        <v>19919719.44406146</v>
       </c>
       <c r="G128">
         <v>231.6868458079414</v>
@@ -3359,7 +3359,7 @@
         <v>2040416955.600668</v>
       </c>
       <c r="F129">
-        <v>2.100669185337662E-11</v>
+        <v>1355612.691685804</v>
       </c>
       <c r="G129">
         <v>293.4277854819478</v>
@@ -3382,7 +3382,7 @@
         <v>1692900626.065979</v>
       </c>
       <c r="F130">
-        <v>-4.048459805865809E-10</v>
+        <v>-26313220.48679258</v>
       </c>
       <c r="G130">
         <v>-103.2671519482615</v>
@@ -3405,7 +3405,7 @@
         <v>1720394457.41666</v>
       </c>
       <c r="F131">
-        <v>1.124581704011619E-09</v>
+        <v>73252353.96180697</v>
       </c>
       <c r="G131">
         <v>-5.629687746690727</v>
@@ -3428,7 +3428,7 @@
         <v>3133499126.051802</v>
       </c>
       <c r="F132">
-        <v>4.056810150157702E-10</v>
+        <v>26487956.92375318</v>
       </c>
       <c r="G132">
         <v>513.8733151715904</v>
@@ -3451,7 +3451,7 @@
         <v>2558647282.837667</v>
       </c>
       <c r="F133">
-        <v>1.324083096971336E-10</v>
+        <v>8682077.774653837</v>
       </c>
       <c r="G133">
         <v>97.41976553934342</v>
@@ -3474,7 +3474,7 @@
         <v>3626362545.983729</v>
       </c>
       <c r="F134">
-        <v>3.329274761910669E-10</v>
+        <v>21895157.18864502</v>
       </c>
       <c r="G134">
         <v>41.18545194646949</v>
@@ -3497,7 +3497,7 @@
         <v>1277680401.84855</v>
       </c>
       <c r="F135">
-        <v>7.848931513077409E-10</v>
+        <v>51875006.56585878</v>
       </c>
       <c r="G135">
         <v>272.9839087463706</v>
@@ -3520,7 +3520,7 @@
         <v>3492410645.778711</v>
       </c>
       <c r="F136">
-        <v>1.151075279461142E-10</v>
+        <v>7629008.36744724</v>
       </c>
       <c r="G136">
         <v>214.870979469381</v>
@@ -3543,7 +3543,7 @@
         <v>2869088868.426933</v>
       </c>
       <c r="F137">
-        <v>-3.204654873402719E-10</v>
+        <v>-21402897.52163912</v>
       </c>
       <c r="G137">
         <v>292.7844131468875</v>
@@ -3566,7 +3566,7 @@
         <v>2928469922.12919</v>
       </c>
       <c r="F138">
-        <v>2.189503996800109E-10</v>
+        <v>14639445.61954908</v>
       </c>
       <c r="G138">
         <v>134.2328068970648</v>
@@ -3589,7 +3589,7 @@
         <v>5881421966.728233</v>
       </c>
       <c r="F139">
-        <v>-6.335002468241721E-10</v>
+        <v>-42492104.45779014</v>
       </c>
       <c r="G139">
         <v>-137.8516154967916</v>
@@ -3612,7 +3612,7 @@
         <v>2618658247.111792</v>
       </c>
       <c r="F140">
-        <v>-2.916639699075257E-10</v>
+        <v>-19895462.42167929</v>
       </c>
       <c r="G140">
         <v>103.8821828568387</v>
@@ -3635,7 +3635,7 @@
         <v>2829358146.408769</v>
       </c>
       <c r="F141">
-        <v>-5.33336779836437E-10</v>
+        <v>-36547100.96472555</v>
       </c>
       <c r="G141">
         <v>353.9091028653904</v>
@@ -3658,7 +3658,7 @@
         <v>3133390673.07931</v>
       </c>
       <c r="F142">
-        <v>-6.603953287429234E-11</v>
+        <v>-4532024.68046705</v>
       </c>
       <c r="G142">
         <v>331.5523769479758</v>
@@ -3681,7 +3681,7 @@
         <v>2764932351.493311</v>
       </c>
       <c r="F143">
-        <v>2.413252796732911E-10</v>
+        <v>16619189.83752748</v>
       </c>
       <c r="G143">
         <v>342.3664263381521</v>
@@ -3704,7 +3704,7 @@
         <v>4044677549.196068</v>
       </c>
       <c r="F144">
-        <v>2.190123043835386E-10</v>
+        <v>15095353.39127744</v>
       </c>
       <c r="G144">
         <v>81.41038431483929</v>
@@ -3727,7 +3727,7 @@
         <v>2093577827.286536</v>
       </c>
       <c r="F145">
-        <v>-5.670829234229884E-10</v>
+        <v>-39141542.31144371</v>
       </c>
       <c r="G145">
         <v>92.47897340587421</v>
@@ -3750,7 +3750,7 @@
         <v>3179222056.615446</v>
       </c>
       <c r="F146">
-        <v>4.196791451277089E-10</v>
+        <v>28992438.82611369</v>
       </c>
       <c r="G146">
         <v>392.0263793176198</v>
@@ -3773,7 +3773,7 @@
         <v>2576563446.582314</v>
       </c>
       <c r="F147">
-        <v>6.422199471601609E-11</v>
+        <v>4456211.232154349</v>
       </c>
       <c r="G147">
         <v>319.5558514401135</v>
@@ -3796,7 +3796,7 @@
         <v>3095424452.912705</v>
       </c>
       <c r="F148">
-        <v>2.286257130076442E-10</v>
+        <v>15887395.34195823</v>
       </c>
       <c r="G148">
         <v>347.1339959839592</v>
@@ -3819,7 +3819,7 @@
         <v>2524462559.141798</v>
       </c>
       <c r="F149">
-        <v>-2.941609397435058E-10</v>
+        <v>-20463206.05191058</v>
       </c>
       <c r="G149">
         <v>219.6700325181319</v>
@@ -3842,7 +3842,7 @@
         <v>2387424251.933375</v>
       </c>
       <c r="F150">
-        <v>-3.056622787269523E-10</v>
+        <v>-21318329.71836824</v>
       </c>
       <c r="G150">
         <v>269.3370609356932</v>
@@ -3865,7 +3865,7 @@
         <v>2609760576.915093</v>
       </c>
       <c r="F151">
-        <v>-3.811380765801864E-10</v>
+        <v>-26807557.21697785</v>
       </c>
       <c r="G151">
         <v>5.522659147667259</v>
@@ -3888,7 +3888,7 @@
         <v>2701662462.370373</v>
       </c>
       <c r="F152">
-        <v>-3.189669041352813E-10</v>
+        <v>-22456878.06023574</v>
       </c>
       <c r="G152">
         <v>430.6616944641905</v>
@@ -3911,7 +3911,7 @@
         <v>2373912766.56643</v>
       </c>
       <c r="F153">
-        <v>-8.912614634881487E-11</v>
+        <v>-6287354.073957154</v>
       </c>
       <c r="G153">
         <v>40.46949130141842</v>
@@ -3934,7 +3934,7 @@
         <v>2288132164.547809</v>
       </c>
       <c r="F154">
-        <v>-7.219945922987928E-10</v>
+        <v>-51227219.09015395</v>
       </c>
       <c r="G154">
         <v>495.9563745355763</v>
@@ -3957,7 +3957,7 @@
         <v>2344624347.877722</v>
       </c>
       <c r="F155">
-        <v>-4.234211905279241E-11</v>
+        <v>-3006011.11654563</v>
       </c>
       <c r="G155">
         <v>191.0072361620598</v>
@@ -3980,7 +3980,7 @@
         <v>2324035744.369361</v>
       </c>
       <c r="F156">
-        <v>5.488826913307117E-10</v>
+        <v>39089639.85088311</v>
       </c>
       <c r="G156">
         <v>36.7033088949083</v>
@@ -4003,7 +4003,7 @@
         <v>1935730441.132565</v>
       </c>
       <c r="F157">
-        <v>-1.675815135048258E-09</v>
+        <v>-120891807.0093691</v>
       </c>
       <c r="G157">
         <v>208.5370214600775</v>
@@ -4026,7 +4026,7 @@
         <v>3128094910.877211</v>
       </c>
       <c r="F158">
-        <v>1.763372648167357E-10</v>
+        <v>12752656.47561182</v>
       </c>
       <c r="G158">
         <v>142.5940394123858</v>
@@ -4049,7 +4049,7 @@
         <v>2985467084.742025</v>
       </c>
       <c r="F159">
-        <v>1.084923343719442E-10</v>
+        <v>7865713.081280822</v>
       </c>
       <c r="G159">
         <v>321.5504153084832</v>
@@ -4072,7 +4072,7 @@
         <v>2539554703.956648</v>
       </c>
       <c r="F160">
-        <v>3.907463806325973E-10</v>
+        <v>28550976.2097047</v>
       </c>
       <c r="G160">
         <v>133.1104821214017</v>
@@ -4095,7 +4095,7 @@
         <v>2122137809.853559</v>
       </c>
       <c r="F161">
-        <v>-9.015688513085777E-10</v>
+        <v>-65936362.86466946</v>
       </c>
       <c r="G161">
         <v>313.5581417605769</v>
@@ -4118,7 +4118,7 @@
         <v>3267782809.83175</v>
       </c>
       <c r="F162">
-        <v>4.464350328870993E-10</v>
+        <v>32685213.94314819</v>
       </c>
       <c r="G162">
         <v>382.7298065708976</v>
@@ -4141,7 +4141,7 @@
         <v>2549208199.796457</v>
       </c>
       <c r="F163">
-        <v>-2.051882167418231E-10</v>
+        <v>-15129787.24873984</v>
       </c>
       <c r="G163">
         <v>116.4342485451196</v>
@@ -4164,7 +4164,7 @@
         <v>2910109884.384812</v>
       </c>
       <c r="F164">
-        <v>1.530663630303746E-10</v>
+        <v>11321095.68117637</v>
       </c>
       <c r="G164">
         <v>430.8414697035229</v>
@@ -4187,7 +4187,7 @@
         <v>3265067322.629371</v>
       </c>
       <c r="F165">
-        <v>-2.988054638535422E-11</v>
+        <v>-2226455.036940136</v>
       </c>
       <c r="G165">
         <v>377.4228902383945</v>
@@ -4210,7 +4210,7 @@
         <v>2365213727.85796</v>
       </c>
       <c r="F166">
-        <v>4.094817074463078E-10</v>
+        <v>30673859.85569298</v>
       </c>
       <c r="G166">
         <v>326.1821565130869</v>
@@ -4233,7 +4233,7 @@
         <v>2429909011.294053</v>
       </c>
       <c r="F167">
-        <v>-2.199021264781797E-10</v>
+        <v>-16523722.63063598</v>
       </c>
       <c r="G167">
         <v>405.6016304391342</v>
@@ -4256,7 +4256,7 @@
         <v>3024902844.993293</v>
       </c>
       <c r="F168">
-        <v>3.521927987838816E-10</v>
+        <v>26526815.54057986</v>
       </c>
       <c r="G168">
         <v>544.7055824357349</v>
@@ -4279,7 +4279,7 @@
         <v>2935604332.999224</v>
       </c>
       <c r="F169">
-        <v>-1.176574806973707E-10</v>
+        <v>-9043179.713305684</v>
       </c>
       <c r="G169">
         <v>70.21986776515132</v>
@@ -4302,7 +4302,7 @@
         <v>2969276017.595953</v>
       </c>
       <c r="F170">
-        <v>5.950467866149234E-10</v>
+        <v>45951324.73962834</v>
       </c>
       <c r="G170">
         <v>118.6938124995394</v>
@@ -4325,7 +4325,7 @@
         <v>2397325331.73465</v>
       </c>
       <c r="F171">
-        <v>-4.544482612844793E-10</v>
+        <v>-35583227.94198732</v>
       </c>
       <c r="G171">
         <v>89.6087900242761</v>
@@ -4348,7 +4348,7 @@
         <v>1090461313.019374</v>
       </c>
       <c r="F172">
-        <v>-1.060146440957569E-09</v>
+        <v>-83037663.30621134</v>
       </c>
       <c r="G172">
         <v>317.188266800946</v>
@@ -4371,7 +4371,7 @@
         <v>505954929.6191821</v>
       </c>
       <c r="F173">
-        <v>-4.029251967199816E-09</v>
+        <v>-315653138.2201879</v>
       </c>
       <c r="G173">
         <v>114.684419813436</v>
@@ -4394,7 +4394,7 @@
         <v>2634097295.423865</v>
       </c>
       <c r="F174">
-        <v>1.798973366163504E-10</v>
+        <v>14186611.91552306</v>
       </c>
       <c r="G174">
         <v>316.651054994061</v>
@@ -4417,7 +4417,7 @@
         <v>2153922306.858066</v>
       </c>
       <c r="F175">
-        <v>-1.304600466675279E-09</v>
+        <v>-104028839.900463</v>
       </c>
       <c r="G175">
         <v>121.3139475424352</v>
@@ -4440,7 +4440,7 @@
         <v>1992678221.439851</v>
       </c>
       <c r="F176">
-        <v>-1.038347356222748E-09</v>
+        <v>-84275469.41572106</v>
       </c>
       <c r="G176">
         <v>-62.16544229493469</v>
@@ -4463,7 +4463,7 @@
         <v>997664084.8940914</v>
       </c>
       <c r="F177">
-        <v>4.072005847793661E-09</v>
+        <v>331335589.3247173</v>
       </c>
       <c r="G177">
         <v>-95.85160748423247</v>
@@ -4486,7 +4486,7 @@
         <v>2738149516.287169</v>
       </c>
       <c r="F178">
-        <v>-6.4026389761196E-11</v>
+        <v>-5315605.952762325</v>
       </c>
       <c r="G178">
         <v>150.1209848485497</v>
@@ -4509,7 +4509,7 @@
         <v>2265164718.023444</v>
       </c>
       <c r="F179">
-        <v>4.6829392949334E-10</v>
+        <v>39205278.65236276</v>
       </c>
       <c r="G179">
         <v>-158.6194640879232</v>
@@ -4532,7 +4532,7 @@
         <v>3196825565.453818</v>
       </c>
       <c r="F180">
-        <v>4.719166991310834E-10</v>
+        <v>39561255.61846042</v>
       </c>
       <c r="G180">
         <v>100.4256205295912</v>
@@ -4555,7 +4555,7 @@
         <v>1499806598.330992</v>
       </c>
       <c r="F181">
-        <v>3.316850923361723E-10</v>
+        <v>27980409.52283004</v>
       </c>
       <c r="G181">
         <v>54.53187711609101</v>
@@ -4578,7 +4578,7 @@
         <v>3471452045.405795</v>
       </c>
       <c r="F182">
-        <v>-3.318219607310964E-10</v>
+        <v>-28622477.40795692</v>
       </c>
       <c r="G182">
         <v>64.7249906789629</v>
@@ -4601,7 +4601,7 @@
         <v>2868653579.087183</v>
       </c>
       <c r="F183">
-        <v>1.083457931360558E-10</v>
+        <v>9407379.650744831</v>
       </c>
       <c r="G183">
         <v>134.4768316275478</v>
@@ -4624,7 +4624,7 @@
         <v>2012332774.739811</v>
       </c>
       <c r="F184">
-        <v>6.049111722535046E-10</v>
+        <v>52585171.57564016</v>
       </c>
       <c r="G184">
         <v>134.4369652716454</v>
@@ -4647,7 +4647,7 @@
         <v>2297603256.137409</v>
       </c>
       <c r="F185">
-        <v>6.288343257074074E-10</v>
+        <v>55151778.96647949</v>
       </c>
       <c r="G185">
         <v>83.61924462412458</v>
@@ -4670,7 +4670,7 @@
         <v>3115670104.780177</v>
       </c>
       <c r="F186">
-        <v>-2.305407778098369E-10</v>
+        <v>-20684258.06144327</v>
       </c>
       <c r="G186">
         <v>93.53874735469434</v>
@@ -4693,7 +4693,7 @@
         <v>2184124492.427251</v>
       </c>
       <c r="F187">
-        <v>6.567791123260811E-10</v>
+        <v>59042938.8992428</v>
       </c>
       <c r="G187">
         <v>34.6268981373526</v>
@@ -4716,7 +4716,7 @@
         <v>2313138605.45255</v>
       </c>
       <c r="F188">
-        <v>1.302105100679028E-10</v>
+        <v>12747770.98337865</v>
       </c>
       <c r="G188">
         <v>111.8581796353327</v>
@@ -4739,7 +4739,7 @@
         <v>2741667337.789729</v>
       </c>
       <c r="F189">
-        <v>3.345608960986932E-10</v>
+        <v>33404815.53269046</v>
       </c>
       <c r="G189">
         <v>-47.22208851763329</v>
@@ -4762,7 +4762,7 @@
         <v>1991439345.439217</v>
       </c>
       <c r="F190">
-        <v>6.984332178580129E-10</v>
+        <v>128796335.2339712</v>
       </c>
       <c r="G190">
         <v>141.7758727360583</v>
@@ -4785,7 +4785,7 @@
         <v>1418031621.297791</v>
       </c>
       <c r="F191">
-        <v>3.702096985279359E-10</v>
+        <v>75556569.19388327</v>
       </c>
       <c r="G191">
         <v>-32.44086179078059</v>
@@ -4808,7 +4808,7 @@
         <v>3644141551.465208</v>
       </c>
       <c r="F192">
-        <v>3.848906338783028E-10</v>
+        <v>85997863.85278149</v>
       </c>
       <c r="G192">
         <v>-67.56613940223765</v>

</xml_diff>

<commit_message>
Fix the doble minus on the third derivate relation
</commit_message>
<xml_diff>
--- a/Project/IAG Solar Flux Atlas/Infrared range/Data/valores_NIR.xlsx
+++ b/Project/IAG Solar Flux Atlas/Infrared range/Data/valores_NIR.xlsx
@@ -438,7 +438,7 @@
         <v>1092414854.350568</v>
       </c>
       <c r="F2">
-        <v>-156677110.1056063</v>
+        <v>156677110.1056063</v>
       </c>
       <c r="G2">
         <v>209.110092138397</v>
@@ -461,7 +461,7 @@
         <v>5206248583.586316</v>
       </c>
       <c r="F3">
-        <v>18519209.4692356</v>
+        <v>-18519209.4692356</v>
       </c>
       <c r="G3">
         <v>363.2835654082753</v>
@@ -484,7 +484,7 @@
         <v>1039916995.203525</v>
       </c>
       <c r="F4">
-        <v>-95784039.45845836</v>
+        <v>95784039.45845836</v>
       </c>
       <c r="G4">
         <v>300.2634136864436</v>
@@ -507,7 +507,7 @@
         <v>680676876.5583919</v>
       </c>
       <c r="F5">
-        <v>-235150854.3567928</v>
+        <v>235150854.3567928</v>
       </c>
       <c r="G5">
         <v>249.632867166849</v>
@@ -530,7 +530,7 @@
         <v>579920772.9419634</v>
       </c>
       <c r="F6">
-        <v>215585189.2373232</v>
+        <v>-215585189.2373232</v>
       </c>
       <c r="G6">
         <v>-118.817428870391</v>
@@ -553,7 +553,7 @@
         <v>2487722571.704799</v>
       </c>
       <c r="F7">
-        <v>-62683098.96488434</v>
+        <v>62683098.96488434</v>
       </c>
       <c r="G7">
         <v>231.1386673049972</v>
@@ -576,7 +576,7 @@
         <v>1164347933.249144</v>
       </c>
       <c r="F8">
-        <v>-166611754.3473985</v>
+        <v>166611754.3473985</v>
       </c>
       <c r="G8">
         <v>53.21822221639219</v>
@@ -599,7 +599,7 @@
         <v>1427904249.565825</v>
       </c>
       <c r="F9">
-        <v>22663026.0553909</v>
+        <v>-22663026.0553909</v>
       </c>
       <c r="G9">
         <v>132.9702376056558</v>
@@ -622,7 +622,7 @@
         <v>4861451483.351841</v>
       </c>
       <c r="F10">
-        <v>28409543.72762407</v>
+        <v>-28409543.72762407</v>
       </c>
       <c r="G10">
         <v>369.2627661837664</v>
@@ -645,7 +645,7 @@
         <v>2369787863.916452</v>
       </c>
       <c r="F11">
-        <v>-45429471.48641107</v>
+        <v>45429471.48641107</v>
       </c>
       <c r="G11">
         <v>221.3481712655098</v>
@@ -668,7 +668,7 @@
         <v>2893465557.268535</v>
       </c>
       <c r="F12">
-        <v>-52285354.05180201</v>
+        <v>52285354.05180201</v>
       </c>
       <c r="G12">
         <v>203.3938889715005</v>
@@ -691,7 +691,7 @@
         <v>4898282972.106872</v>
       </c>
       <c r="F13">
-        <v>7300468.186603961</v>
+        <v>-7300468.186603961</v>
       </c>
       <c r="G13">
         <v>440.04664022485</v>
@@ -714,7 +714,7 @@
         <v>4769684636.022537</v>
       </c>
       <c r="F14">
-        <v>-3783279.059394291</v>
+        <v>3783279.059394291</v>
       </c>
       <c r="G14">
         <v>196.5138348174656</v>
@@ -737,7 +737,7 @@
         <v>1175894603.604178</v>
       </c>
       <c r="F15">
-        <v>-101648915.6019635</v>
+        <v>101648915.6019635</v>
       </c>
       <c r="G15">
         <v>163.5013882968728</v>
@@ -760,7 +760,7 @@
         <v>517253609.0199448</v>
       </c>
       <c r="F16">
-        <v>35809794.85313801</v>
+        <v>-35809794.85313801</v>
       </c>
       <c r="G16">
         <v>58.2879763077196</v>
@@ -783,7 +783,7 @@
         <v>651237286.9919277</v>
       </c>
       <c r="F17">
-        <v>-406184614.3090176</v>
+        <v>406184614.3090176</v>
       </c>
       <c r="G17">
         <v>55.24638439732712</v>
@@ -806,7 +806,7 @@
         <v>1483377073.555127</v>
       </c>
       <c r="F18">
-        <v>-87995685.52016665</v>
+        <v>87995685.52016665</v>
       </c>
       <c r="G18">
         <v>240.7584556362024</v>
@@ -829,7 +829,7 @@
         <v>5741618897.409628</v>
       </c>
       <c r="F19">
-        <v>-3332097.627462617</v>
+        <v>3332097.627462617</v>
       </c>
       <c r="G19">
         <v>234.7626117048913</v>
@@ -852,7 +852,7 @@
         <v>816452194.0869088</v>
       </c>
       <c r="F20">
-        <v>-24187923.80759507</v>
+        <v>24187923.80759507</v>
       </c>
       <c r="G20">
         <v>78.22169691553601</v>
@@ -875,7 +875,7 @@
         <v>3023016423.668905</v>
       </c>
       <c r="F21">
-        <v>-977415.4649770735</v>
+        <v>977415.4649770735</v>
       </c>
       <c r="G21">
         <v>211.4314352049752</v>
@@ -898,7 +898,7 @@
         <v>2268074095.879919</v>
       </c>
       <c r="F22">
-        <v>-51229562.94007045</v>
+        <v>51229562.94007045</v>
       </c>
       <c r="G22">
         <v>188.1546650230045</v>
@@ -921,7 +921,7 @@
         <v>1167710602.469932</v>
       </c>
       <c r="F23">
-        <v>-101261740.0364153</v>
+        <v>101261740.0364153</v>
       </c>
       <c r="G23">
         <v>156.1789013206684</v>
@@ -944,7 +944,7 @@
         <v>2620537720.623078</v>
       </c>
       <c r="F24">
-        <v>-8616107.045082089</v>
+        <v>8616107.045082089</v>
       </c>
       <c r="G24">
         <v>150.158336158803</v>
@@ -967,7 +967,7 @@
         <v>912103665.3756156</v>
       </c>
       <c r="F25">
-        <v>-155365542.5129987</v>
+        <v>155365542.5129987</v>
       </c>
       <c r="G25">
         <v>201.9466609972183</v>
@@ -990,7 +990,7 @@
         <v>6334397162.849628</v>
       </c>
       <c r="F26">
-        <v>5619379.032977202</v>
+        <v>-5619379.032977202</v>
       </c>
       <c r="G26">
         <v>242.1715747933119</v>
@@ -1013,7 +1013,7 @@
         <v>2907342842.092541</v>
       </c>
       <c r="F27">
-        <v>-23491007.64812877</v>
+        <v>23491007.64812877</v>
       </c>
       <c r="G27">
         <v>238.6633748817404</v>
@@ -1036,7 +1036,7 @@
         <v>3650308171.970758</v>
       </c>
       <c r="F28">
-        <v>4861517.001753004</v>
+        <v>-4861517.001753004</v>
       </c>
       <c r="G28">
         <v>209.894352961243</v>
@@ -1059,7 +1059,7 @@
         <v>5367784831.088258</v>
       </c>
       <c r="F29">
-        <v>7306275.050283175</v>
+        <v>-7306275.050283175</v>
       </c>
       <c r="G29">
         <v>437.9865704075818</v>
@@ -1082,7 +1082,7 @@
         <v>5502191211.121552</v>
       </c>
       <c r="F30">
-        <v>-3667309.38911736</v>
+        <v>3667309.38911736</v>
       </c>
       <c r="G30">
         <v>338.6320776117072</v>
@@ -1105,7 +1105,7 @@
         <v>1109103792.656712</v>
       </c>
       <c r="F31">
-        <v>-25102531.12714076</v>
+        <v>25102531.12714076</v>
       </c>
       <c r="G31">
         <v>164.6814456252225</v>
@@ -1128,7 +1128,7 @@
         <v>2276211567.059862</v>
       </c>
       <c r="F32">
-        <v>-23994375.32402267</v>
+        <v>23994375.32402267</v>
       </c>
       <c r="G32">
         <v>277.6895329283418</v>
@@ -1151,7 +1151,7 @@
         <v>2230216978.745636</v>
       </c>
       <c r="F33">
-        <v>-28263552.39839941</v>
+        <v>28263552.39839941</v>
       </c>
       <c r="G33">
         <v>175.0261407137777</v>
@@ -1174,7 +1174,7 @@
         <v>4012371034.929343</v>
       </c>
       <c r="F34">
-        <v>-9957776.974086111</v>
+        <v>9957776.974086111</v>
       </c>
       <c r="G34">
         <v>253.6373431923298</v>
@@ -1197,7 +1197,7 @@
         <v>1423530335.532048</v>
       </c>
       <c r="F35">
-        <v>-48341681.80190385</v>
+        <v>48341681.80190385</v>
       </c>
       <c r="G35">
         <v>294.6869318163317</v>
@@ -1220,7 +1220,7 @@
         <v>5131435504.372919</v>
       </c>
       <c r="F36">
-        <v>-8438671.782919452</v>
+        <v>8438671.782919452</v>
       </c>
       <c r="G36">
         <v>208.4593297016262</v>
@@ -1243,7 +1243,7 @@
         <v>3567627233.572556</v>
       </c>
       <c r="F37">
-        <v>-13690480.77423065</v>
+        <v>13690480.77423065</v>
       </c>
       <c r="G37">
         <v>257.6479066640685</v>
@@ -1266,7 +1266,7 @@
         <v>3740177205.343518</v>
       </c>
       <c r="F38">
-        <v>-5682019.626809872</v>
+        <v>5682019.626809872</v>
       </c>
       <c r="G38">
         <v>278.1147539102653</v>
@@ -1289,7 +1289,7 @@
         <v>4551789703.786042</v>
       </c>
       <c r="F39">
-        <v>7373565.200082134</v>
+        <v>-7373565.200082134</v>
       </c>
       <c r="G39">
         <v>228.2972618982217</v>
@@ -1312,7 +1312,7 @@
         <v>3735533218.436416</v>
       </c>
       <c r="F40">
-        <v>-58420175.82534759</v>
+        <v>58420175.82534759</v>
       </c>
       <c r="G40">
         <v>-78.82258140793543</v>
@@ -1335,7 +1335,7 @@
         <v>5920332872.86448</v>
       </c>
       <c r="F41">
-        <v>8343150.216613088</v>
+        <v>-8343150.216613088</v>
       </c>
       <c r="G41">
         <v>293.786195995636</v>
@@ -1358,7 +1358,7 @@
         <v>1719662461.027918</v>
       </c>
       <c r="F42">
-        <v>17818425.38171053</v>
+        <v>-17818425.38171053</v>
       </c>
       <c r="G42">
         <v>60.52873280376289</v>
@@ -1381,7 +1381,7 @@
         <v>2052153873.602626</v>
       </c>
       <c r="F43">
-        <v>-6126794.508152236</v>
+        <v>6126794.508152236</v>
       </c>
       <c r="G43">
         <v>84.10917700767887</v>
@@ -1404,7 +1404,7 @@
         <v>5053048059.109766</v>
       </c>
       <c r="F44">
-        <v>-29709112.09872661</v>
+        <v>29709112.09872661</v>
       </c>
       <c r="G44">
         <v>195.1901477600028</v>
@@ -1427,7 +1427,7 @@
         <v>4078361117.601238</v>
       </c>
       <c r="F45">
-        <v>33204587.71600025</v>
+        <v>-33204587.71600025</v>
       </c>
       <c r="G45">
         <v>448.9066877308219</v>
@@ -1450,7 +1450,7 @@
         <v>3234104353.83377</v>
       </c>
       <c r="F46">
-        <v>7962682.93565054</v>
+        <v>-7962682.93565054</v>
       </c>
       <c r="G46">
         <v>161.3177175190825</v>
@@ -1473,7 +1473,7 @@
         <v>3292310950.058791</v>
       </c>
       <c r="F47">
-        <v>8322813.517383904</v>
+        <v>-8322813.517383904</v>
       </c>
       <c r="G47">
         <v>213.8464966395116</v>
@@ -1496,7 +1496,7 @@
         <v>484919102.1449975</v>
       </c>
       <c r="F48">
-        <v>37658692.86906283</v>
+        <v>-37658692.86906283</v>
       </c>
       <c r="G48">
         <v>-51.88218762412625</v>
@@ -1519,7 +1519,7 @@
         <v>1956128998.876171</v>
       </c>
       <c r="F49">
-        <v>-63107876.30689377</v>
+        <v>63107876.30689377</v>
       </c>
       <c r="G49">
         <v>68.71090987194373</v>
@@ -1542,7 +1542,7 @@
         <v>3958370237.736347</v>
       </c>
       <c r="F50">
-        <v>-7461850.332053294</v>
+        <v>7461850.332053294</v>
       </c>
       <c r="G50">
         <v>213.2540066162134</v>
@@ -1565,7 +1565,7 @@
         <v>885320110.7129227</v>
       </c>
       <c r="F51">
-        <v>18408945.50113069</v>
+        <v>-18408945.50113069</v>
       </c>
       <c r="G51">
         <v>55.85954716125617</v>
@@ -1588,7 +1588,7 @@
         <v>2893479150.314776</v>
       </c>
       <c r="F52">
-        <v>-25835291.56025861</v>
+        <v>25835291.56025861</v>
       </c>
       <c r="G52">
         <v>281.6710125485241</v>
@@ -1611,7 +1611,7 @@
         <v>856868878.490669</v>
       </c>
       <c r="F53">
-        <v>-126876111.3540012</v>
+        <v>126876111.3540012</v>
       </c>
       <c r="G53">
         <v>359.3501419186555</v>
@@ -1634,7 +1634,7 @@
         <v>3698188201.947296</v>
       </c>
       <c r="F54">
-        <v>-7148187.431506136</v>
+        <v>7148187.431506136</v>
       </c>
       <c r="G54">
         <v>221.9724054358576</v>
@@ -1657,7 +1657,7 @@
         <v>2922384018.712894</v>
       </c>
       <c r="F55">
-        <v>8848614.204445509</v>
+        <v>-8848614.204445509</v>
       </c>
       <c r="G55">
         <v>225.6869093191555</v>
@@ -1680,7 +1680,7 @@
         <v>4279152310.849101</v>
       </c>
       <c r="F56">
-        <v>4111393.746382472</v>
+        <v>-4111393.746382472</v>
       </c>
       <c r="G56">
         <v>350.9627206966982</v>
@@ -1703,7 +1703,7 @@
         <v>2966110426.167465</v>
       </c>
       <c r="F57">
-        <v>68640944.86805318</v>
+        <v>-68640944.86805318</v>
       </c>
       <c r="G57">
         <v>-127.9523652009337</v>
@@ -1726,7 +1726,7 @@
         <v>3337081972.08334</v>
       </c>
       <c r="F58">
-        <v>-12799969.90510492</v>
+        <v>12799969.90510492</v>
       </c>
       <c r="G58">
         <v>334.645859331857</v>
@@ -1749,7 +1749,7 @@
         <v>2273626482.28181</v>
       </c>
       <c r="F59">
-        <v>-4101617.602997416</v>
+        <v>4101617.602997416</v>
       </c>
       <c r="G59">
         <v>236.03185496702</v>
@@ -1772,7 +1772,7 @@
         <v>1663237571.869143</v>
       </c>
       <c r="F60">
-        <v>-24495923.06465667</v>
+        <v>24495923.06465667</v>
       </c>
       <c r="G60">
         <v>315.1020603992357</v>
@@ -1795,7 +1795,7 @@
         <v>5652830475.671362</v>
       </c>
       <c r="F61">
-        <v>650730.1445753785</v>
+        <v>-650730.1445753785</v>
       </c>
       <c r="G61">
         <v>269.930418796854</v>
@@ -1818,7 +1818,7 @@
         <v>1054536340.142622</v>
       </c>
       <c r="F62">
-        <v>-215975076.2760331</v>
+        <v>215975076.2760331</v>
       </c>
       <c r="G62">
         <v>171.488168777924</v>
@@ -1841,7 +1841,7 @@
         <v>3940752423.939021</v>
       </c>
       <c r="F63">
-        <v>17138920.22262292</v>
+        <v>-17138920.22262292</v>
       </c>
       <c r="G63">
         <v>170.5938907839318</v>
@@ -1864,7 +1864,7 @@
         <v>3645317858.151546</v>
       </c>
       <c r="F64">
-        <v>27702535.8647331</v>
+        <v>-27702535.8647331</v>
       </c>
       <c r="G64">
         <v>273.0316685858902</v>
@@ -1887,7 +1887,7 @@
         <v>4176362792.286147</v>
       </c>
       <c r="F65">
-        <v>-11991303.16024815</v>
+        <v>11991303.16024815</v>
       </c>
       <c r="G65">
         <v>-22.26326037205379</v>
@@ -1910,7 +1910,7 @@
         <v>2510051758.391216</v>
       </c>
       <c r="F66">
-        <v>23559156.52719074</v>
+        <v>-23559156.52719074</v>
       </c>
       <c r="G66">
         <v>-142.8399188742064</v>
@@ -1933,7 +1933,7 @@
         <v>3416335965.676072</v>
       </c>
       <c r="F67">
-        <v>4225147.812217094</v>
+        <v>-4225147.812217094</v>
       </c>
       <c r="G67">
         <v>210.4124623500545</v>
@@ -1956,7 +1956,7 @@
         <v>5251662869.876287</v>
       </c>
       <c r="F68">
-        <v>56996246.20949438</v>
+        <v>-56996246.20949438</v>
       </c>
       <c r="G68">
         <v>43.98963272055954</v>
@@ -1979,7 +1979,7 @@
         <v>2350162102.19848</v>
       </c>
       <c r="F69">
-        <v>-18432425.35255145</v>
+        <v>18432425.35255145</v>
       </c>
       <c r="G69">
         <v>283.3915436144903</v>
@@ -2002,7 +2002,7 @@
         <v>3532133521.254247</v>
       </c>
       <c r="F70">
-        <v>19652248.51544683</v>
+        <v>-19652248.51544683</v>
       </c>
       <c r="G70">
         <v>346.4689432125126</v>
@@ -2025,7 +2025,7 @@
         <v>3476608258.668179</v>
       </c>
       <c r="F71">
-        <v>-1998760.828410971</v>
+        <v>1998760.828410971</v>
       </c>
       <c r="G71">
         <v>75.45033175572252</v>
@@ -2048,7 +2048,7 @@
         <v>3258857784.176424</v>
       </c>
       <c r="F72">
-        <v>9281268.46865187</v>
+        <v>-9281268.46865187</v>
       </c>
       <c r="G72">
         <v>182.3348335479448</v>
@@ -2071,7 +2071,7 @@
         <v>1854800454.515697</v>
       </c>
       <c r="F73">
-        <v>39080523.23495647</v>
+        <v>-39080523.23495647</v>
       </c>
       <c r="G73">
         <v>69.11817059749109</v>
@@ -2094,7 +2094,7 @@
         <v>3705141813.06572</v>
       </c>
       <c r="F74">
-        <v>23251624.81021379</v>
+        <v>-23251624.81021379</v>
       </c>
       <c r="G74">
         <v>277.8832990826441</v>
@@ -2117,7 +2117,7 @@
         <v>3223982704.849172</v>
       </c>
       <c r="F75">
-        <v>14905797.98844591</v>
+        <v>-14905797.98844591</v>
       </c>
       <c r="G75">
         <v>387.9398314054862</v>
@@ -2140,7 +2140,7 @@
         <v>2355292363.132841</v>
       </c>
       <c r="F76">
-        <v>4009330.396214958</v>
+        <v>-4009330.396214958</v>
       </c>
       <c r="G76">
         <v>157.4861582376646</v>
@@ -2163,7 +2163,7 @@
         <v>3630380395.531632</v>
       </c>
       <c r="F77">
-        <v>18025201.92779333</v>
+        <v>-18025201.92779333</v>
       </c>
       <c r="G77">
         <v>334.2137252694796</v>
@@ -2186,7 +2186,7 @@
         <v>1107639082.173041</v>
       </c>
       <c r="F78">
-        <v>260580081.1625765</v>
+        <v>-260580081.1625765</v>
       </c>
       <c r="G78">
         <v>102.2198540424131</v>
@@ -2209,7 +2209,7 @@
         <v>3322326761.809361</v>
       </c>
       <c r="F79">
-        <v>-6520566.126871623</v>
+        <v>6520566.126871623</v>
       </c>
       <c r="G79">
         <v>485.4007268146134</v>
@@ -2232,7 +2232,7 @@
         <v>674786405.2326441</v>
       </c>
       <c r="F80">
-        <v>-1157440.795803524</v>
+        <v>1157440.795803524</v>
       </c>
       <c r="G80">
         <v>3.918767101372705</v>
@@ -2255,7 +2255,7 @@
         <v>3256569347.414473</v>
       </c>
       <c r="F81">
-        <v>-20886780.63261012</v>
+        <v>20886780.63261012</v>
       </c>
       <c r="G81">
         <v>537.452358866126</v>
@@ -2278,7 +2278,7 @@
         <v>2755933012.006021</v>
       </c>
       <c r="F82">
-        <v>40158856.45263437</v>
+        <v>-40158856.45263437</v>
       </c>
       <c r="G82">
         <v>101.5716236259524</v>
@@ -2301,7 +2301,7 @@
         <v>1496411122.723968</v>
       </c>
       <c r="F83">
-        <v>-102506662.6875892</v>
+        <v>102506662.6875892</v>
       </c>
       <c r="G83">
         <v>243.7876290177686</v>
@@ -2324,7 +2324,7 @@
         <v>1369355575.743196</v>
       </c>
       <c r="F84">
-        <v>-99287991.6351856</v>
+        <v>99287991.6351856</v>
       </c>
       <c r="G84">
         <v>251.1387476538749</v>
@@ -2347,7 +2347,7 @@
         <v>1331376628.093632</v>
       </c>
       <c r="F85">
-        <v>-59480893.18530277</v>
+        <v>59480893.18530277</v>
       </c>
       <c r="G85">
         <v>46.34888772717395</v>
@@ -2370,7 +2370,7 @@
         <v>3060273067.410341</v>
       </c>
       <c r="F86">
-        <v>11301427.42831764</v>
+        <v>-11301427.42831764</v>
       </c>
       <c r="G86">
         <v>175.5993074487081</v>
@@ -2393,7 +2393,7 @@
         <v>3785816998.200178</v>
       </c>
       <c r="F87">
-        <v>15407605.52427121</v>
+        <v>-15407605.52427121</v>
       </c>
       <c r="G87">
         <v>191.0060096595961</v>
@@ -2416,7 +2416,7 @@
         <v>3349839984.879492</v>
       </c>
       <c r="F88">
-        <v>-11518568.90202348</v>
+        <v>11518568.90202348</v>
       </c>
       <c r="G88">
         <v>-7.713523254235525</v>
@@ -2439,7 +2439,7 @@
         <v>2115502168.66674</v>
       </c>
       <c r="F89">
-        <v>18044504.93170052</v>
+        <v>-18044504.93170052</v>
       </c>
       <c r="G89">
         <v>304.5009523394917</v>
@@ -2462,7 +2462,7 @@
         <v>1727811374.925148</v>
       </c>
       <c r="F90">
-        <v>-40216141.81642985</v>
+        <v>40216141.81642985</v>
       </c>
       <c r="G90">
         <v>336.9323512893235</v>
@@ -2485,7 +2485,7 @@
         <v>3345003900.470722</v>
       </c>
       <c r="F91">
-        <v>-7466818.371781709</v>
+        <v>7466818.371781709</v>
       </c>
       <c r="G91">
         <v>-34.60802334615429</v>
@@ -2508,7 +2508,7 @@
         <v>1763419783.923234</v>
       </c>
       <c r="F92">
-        <v>-57039602.0169448</v>
+        <v>57039602.0169448</v>
       </c>
       <c r="G92">
         <v>272.9875613605734</v>
@@ -2531,7 +2531,7 @@
         <v>641019393.6751802</v>
       </c>
       <c r="F93">
-        <v>-176514311.1066101</v>
+        <v>176514311.1066101</v>
       </c>
       <c r="G93">
         <v>265.147676599972</v>
@@ -2554,7 +2554,7 @@
         <v>2128410984.442255</v>
       </c>
       <c r="F94">
-        <v>29292744.5491517</v>
+        <v>-29292744.5491517</v>
       </c>
       <c r="G94">
         <v>247.660755848954</v>
@@ -2577,7 +2577,7 @@
         <v>1920806518.761335</v>
       </c>
       <c r="F95">
-        <v>14444204.9751977</v>
+        <v>-14444204.9751977</v>
       </c>
       <c r="G95">
         <v>99.81629483784745</v>
@@ -2600,7 +2600,7 @@
         <v>3308374422.757637</v>
       </c>
       <c r="F96">
-        <v>12927320.51711405</v>
+        <v>-12927320.51711405</v>
       </c>
       <c r="G96">
         <v>368.3630993007404</v>
@@ -2623,7 +2623,7 @@
         <v>3708052043.393218</v>
       </c>
       <c r="F97">
-        <v>15545737.79064793</v>
+        <v>-15545737.79064793</v>
       </c>
       <c r="G97">
         <v>230.0753746088103</v>
@@ -2646,7 +2646,7 @@
         <v>1337421639.484831</v>
       </c>
       <c r="F98">
-        <v>-12035485.47258861</v>
+        <v>12035485.47258861</v>
       </c>
       <c r="G98">
         <v>114.9415798028418</v>
@@ -2669,7 +2669,7 @@
         <v>3638577979.461855</v>
       </c>
       <c r="F99">
-        <v>5329848.285221979</v>
+        <v>-5329848.285221979</v>
       </c>
       <c r="G99">
         <v>42.13583432360907</v>
@@ -2692,7 +2692,7 @@
         <v>2776986058.737023</v>
       </c>
       <c r="F100">
-        <v>5524094.789445193</v>
+        <v>-5524094.789445193</v>
       </c>
       <c r="G100">
         <v>271.8919236143388</v>
@@ -2715,7 +2715,7 @@
         <v>3431266749.599977</v>
       </c>
       <c r="F101">
-        <v>6144866.720842819</v>
+        <v>-6144866.720842819</v>
       </c>
       <c r="G101">
         <v>256.424267459517</v>
@@ -2738,7 +2738,7 @@
         <v>2161430199.950818</v>
       </c>
       <c r="F102">
-        <v>39521753.0038707</v>
+        <v>-39521753.0038707</v>
       </c>
       <c r="G102">
         <v>53.57015187109182</v>
@@ -2761,7 +2761,7 @@
         <v>2958394824.958137</v>
       </c>
       <c r="F103">
-        <v>-130391513.3155631</v>
+        <v>130391513.3155631</v>
       </c>
       <c r="G103">
         <v>30.58936425919826</v>
@@ -2784,7 +2784,7 @@
         <v>3358313621.082551</v>
       </c>
       <c r="F104">
-        <v>940112.4217698813</v>
+        <v>-940112.4217698813</v>
       </c>
       <c r="G104">
         <v>281.0230382164584</v>
@@ -2807,7 +2807,7 @@
         <v>1497438084.829989</v>
       </c>
       <c r="F105">
-        <v>13984483.06792466</v>
+        <v>-13984483.06792466</v>
       </c>
       <c r="G105">
         <v>309.6002183101011</v>
@@ -2830,7 +2830,7 @@
         <v>3691882257.913296</v>
       </c>
       <c r="F106">
-        <v>-70925485.27770038</v>
+        <v>70925485.27770038</v>
       </c>
       <c r="G106">
         <v>43.94458190379509</v>
@@ -2853,7 +2853,7 @@
         <v>3389258173.328023</v>
       </c>
       <c r="F107">
-        <v>13139329.48703831</v>
+        <v>-13139329.48703831</v>
       </c>
       <c r="G107">
         <v>374.3551108861444</v>
@@ -2876,7 +2876,7 @@
         <v>3360735596.695724</v>
       </c>
       <c r="F108">
-        <v>1424466.953564628</v>
+        <v>-1424466.953564628</v>
       </c>
       <c r="G108">
         <v>249.7017225159084</v>
@@ -2899,7 +2899,7 @@
         <v>2775194890.509315</v>
       </c>
       <c r="F109">
-        <v>46096031.02674194</v>
+        <v>-46096031.02674194</v>
       </c>
       <c r="G109">
         <v>98.80106273223207</v>
@@ -2922,7 +2922,7 @@
         <v>3272568222.625025</v>
       </c>
       <c r="F110">
-        <v>1256206.585799897</v>
+        <v>-1256206.585799897</v>
       </c>
       <c r="G110">
         <v>324.5962672596718</v>
@@ -2945,7 +2945,7 @@
         <v>853750483.476817</v>
       </c>
       <c r="F111">
-        <v>23232924.08383252</v>
+        <v>-23232924.08383252</v>
       </c>
       <c r="G111">
         <v>-7.584593315247607</v>
@@ -2968,7 +2968,7 @@
         <v>1984738847.859315</v>
       </c>
       <c r="F112">
-        <v>3376419.004386254</v>
+        <v>-3376419.004386254</v>
       </c>
       <c r="G112">
         <v>100.4300806716848</v>
@@ -2991,7 +2991,7 @@
         <v>2977581355.170902</v>
       </c>
       <c r="F113">
-        <v>4201763.757616004</v>
+        <v>-4201763.757616004</v>
       </c>
       <c r="G113">
         <v>414.9451478422461</v>
@@ -3014,7 +3014,7 @@
         <v>2551710361.498037</v>
       </c>
       <c r="F114">
-        <v>-25374146.47156611</v>
+        <v>25374146.47156611</v>
       </c>
       <c r="G114">
         <v>208.4068130961335</v>
@@ -3037,7 +3037,7 @@
         <v>2189644938.355878</v>
       </c>
       <c r="F115">
-        <v>-17936058.31621805</v>
+        <v>17936058.31621805</v>
       </c>
       <c r="G115">
         <v>172.3812270593169</v>
@@ -3060,7 +3060,7 @@
         <v>4022960594.522149</v>
       </c>
       <c r="F116">
-        <v>-12832525.2108562</v>
+        <v>12832525.2108562</v>
       </c>
       <c r="G116">
         <v>225.4058009455241</v>
@@ -3083,7 +3083,7 @@
         <v>3121919735.65976</v>
       </c>
       <c r="F117">
-        <v>-2315641.968682407</v>
+        <v>2315641.968682407</v>
       </c>
       <c r="G117">
         <v>431.5333003021923</v>
@@ -3106,7 +3106,7 @@
         <v>1535985471.910607</v>
       </c>
       <c r="F118">
-        <v>75078379.31545964</v>
+        <v>-75078379.31545964</v>
       </c>
       <c r="G118">
         <v>361.3889672487713</v>
@@ -3129,7 +3129,7 @@
         <v>1731865508.150192</v>
       </c>
       <c r="F119">
-        <v>73051761.23565413</v>
+        <v>-73051761.23565413</v>
       </c>
       <c r="G119">
         <v>1.890522443555685</v>
@@ -3152,7 +3152,7 @@
         <v>3139864006.512664</v>
       </c>
       <c r="F120">
-        <v>26694836.80401955</v>
+        <v>-26694836.80401955</v>
       </c>
       <c r="G120">
         <v>360.8531826447532</v>
@@ -3175,7 +3175,7 @@
         <v>972403926.8396584</v>
       </c>
       <c r="F121">
-        <v>-289160107.4694867</v>
+        <v>289160107.4694867</v>
       </c>
       <c r="G121">
         <v>253.149067868522</v>
@@ -3198,7 +3198,7 @@
         <v>3555038684.349282</v>
       </c>
       <c r="F122">
-        <v>11382656.53319679</v>
+        <v>-11382656.53319679</v>
       </c>
       <c r="G122">
         <v>330.5243848898632</v>
@@ -3221,7 +3221,7 @@
         <v>3312740761.39504</v>
       </c>
       <c r="F123">
-        <v>-7834604.476762424</v>
+        <v>7834604.476762424</v>
       </c>
       <c r="G123">
         <v>166.1026827974451</v>
@@ -3244,7 +3244,7 @@
         <v>1441603979.621701</v>
       </c>
       <c r="F124">
-        <v>116512923.8326921</v>
+        <v>-116512923.8326921</v>
       </c>
       <c r="G124">
         <v>248.9546179611329</v>
@@ -3267,7 +3267,7 @@
         <v>3151944383.743469</v>
       </c>
       <c r="F125">
-        <v>-7595046.538135923</v>
+        <v>7595046.538135923</v>
       </c>
       <c r="G125">
         <v>328.0835720292703</v>
@@ -3290,7 +3290,7 @@
         <v>2723534864.191213</v>
       </c>
       <c r="F126">
-        <v>9337295.743194398</v>
+        <v>-9337295.743194398</v>
       </c>
       <c r="G126">
         <v>82.93084284040249</v>
@@ -3313,7 +3313,7 @@
         <v>3508808338.613146</v>
       </c>
       <c r="F127">
-        <v>34674361.21255974</v>
+        <v>-34674361.21255974</v>
       </c>
       <c r="G127">
         <v>258.1430529977978</v>
@@ -3336,7 +3336,7 @@
         <v>3318848889.865634</v>
       </c>
       <c r="F128">
-        <v>19919719.44406146</v>
+        <v>-19919719.44406146</v>
       </c>
       <c r="G128">
         <v>231.6868458079414</v>
@@ -3359,7 +3359,7 @@
         <v>2040416955.600668</v>
       </c>
       <c r="F129">
-        <v>1355612.691685804</v>
+        <v>-1355612.691685804</v>
       </c>
       <c r="G129">
         <v>293.4277854819478</v>
@@ -3382,7 +3382,7 @@
         <v>1692900626.065979</v>
       </c>
       <c r="F130">
-        <v>-26313220.48679258</v>
+        <v>26313220.48679258</v>
       </c>
       <c r="G130">
         <v>-103.2671519482615</v>
@@ -3405,7 +3405,7 @@
         <v>1720394457.41666</v>
       </c>
       <c r="F131">
-        <v>73252353.96180697</v>
+        <v>-73252353.96180697</v>
       </c>
       <c r="G131">
         <v>-5.629687746690727</v>
@@ -3428,7 +3428,7 @@
         <v>3133499126.051802</v>
       </c>
       <c r="F132">
-        <v>26487956.92375318</v>
+        <v>-26487956.92375318</v>
       </c>
       <c r="G132">
         <v>513.8733151715904</v>
@@ -3451,7 +3451,7 @@
         <v>2558647282.837667</v>
       </c>
       <c r="F133">
-        <v>8682077.774653837</v>
+        <v>-8682077.774653837</v>
       </c>
       <c r="G133">
         <v>97.41976553934342</v>
@@ -3474,7 +3474,7 @@
         <v>3626362545.983729</v>
       </c>
       <c r="F134">
-        <v>21895157.18864502</v>
+        <v>-21895157.18864502</v>
       </c>
       <c r="G134">
         <v>41.18545194646949</v>
@@ -3497,7 +3497,7 @@
         <v>1277680401.84855</v>
       </c>
       <c r="F135">
-        <v>51875006.56585878</v>
+        <v>-51875006.56585878</v>
       </c>
       <c r="G135">
         <v>272.9839087463706</v>
@@ -3520,7 +3520,7 @@
         <v>3492410645.778711</v>
       </c>
       <c r="F136">
-        <v>7629008.36744724</v>
+        <v>-7629008.36744724</v>
       </c>
       <c r="G136">
         <v>214.870979469381</v>
@@ -3543,7 +3543,7 @@
         <v>2869088868.426933</v>
       </c>
       <c r="F137">
-        <v>-21402897.52163912</v>
+        <v>21402897.52163912</v>
       </c>
       <c r="G137">
         <v>292.7844131468875</v>
@@ -3566,7 +3566,7 @@
         <v>2928469922.12919</v>
       </c>
       <c r="F138">
-        <v>14639445.61954908</v>
+        <v>-14639445.61954908</v>
       </c>
       <c r="G138">
         <v>134.2328068970648</v>
@@ -3589,7 +3589,7 @@
         <v>5881421966.728233</v>
       </c>
       <c r="F139">
-        <v>-42492104.45779014</v>
+        <v>42492104.45779014</v>
       </c>
       <c r="G139">
         <v>-137.8516154967916</v>
@@ -3612,7 +3612,7 @@
         <v>2618658247.111792</v>
       </c>
       <c r="F140">
-        <v>-19895462.42167929</v>
+        <v>19895462.42167929</v>
       </c>
       <c r="G140">
         <v>103.8821828568387</v>
@@ -3635,7 +3635,7 @@
         <v>2829358146.408769</v>
       </c>
       <c r="F141">
-        <v>-36547100.96472555</v>
+        <v>36547100.96472555</v>
       </c>
       <c r="G141">
         <v>353.9091028653904</v>
@@ -3658,7 +3658,7 @@
         <v>3133390673.07931</v>
       </c>
       <c r="F142">
-        <v>-4532024.68046705</v>
+        <v>4532024.68046705</v>
       </c>
       <c r="G142">
         <v>331.5523769479758</v>
@@ -3681,7 +3681,7 @@
         <v>2764932351.493311</v>
       </c>
       <c r="F143">
-        <v>16619189.83752748</v>
+        <v>-16619189.83752748</v>
       </c>
       <c r="G143">
         <v>342.3664263381521</v>
@@ -3704,7 +3704,7 @@
         <v>4044677549.196068</v>
       </c>
       <c r="F144">
-        <v>15095353.39127744</v>
+        <v>-15095353.39127744</v>
       </c>
       <c r="G144">
         <v>81.41038431483929</v>
@@ -3727,7 +3727,7 @@
         <v>2093577827.286536</v>
       </c>
       <c r="F145">
-        <v>-39141542.31144371</v>
+        <v>39141542.31144371</v>
       </c>
       <c r="G145">
         <v>92.47897340587421</v>
@@ -3750,7 +3750,7 @@
         <v>3179222056.615446</v>
       </c>
       <c r="F146">
-        <v>28992438.82611369</v>
+        <v>-28992438.82611369</v>
       </c>
       <c r="G146">
         <v>392.0263793176198</v>
@@ -3773,7 +3773,7 @@
         <v>2576563446.582314</v>
       </c>
       <c r="F147">
-        <v>4456211.232154349</v>
+        <v>-4456211.232154349</v>
       </c>
       <c r="G147">
         <v>319.5558514401135</v>
@@ -3796,7 +3796,7 @@
         <v>3095424452.912705</v>
       </c>
       <c r="F148">
-        <v>15887395.34195823</v>
+        <v>-15887395.34195823</v>
       </c>
       <c r="G148">
         <v>347.1339959839592</v>
@@ -3819,7 +3819,7 @@
         <v>2524462559.141798</v>
       </c>
       <c r="F149">
-        <v>-20463206.05191058</v>
+        <v>20463206.05191058</v>
       </c>
       <c r="G149">
         <v>219.6700325181319</v>
@@ -3842,7 +3842,7 @@
         <v>2387424251.933375</v>
       </c>
       <c r="F150">
-        <v>-21318329.71836824</v>
+        <v>21318329.71836824</v>
       </c>
       <c r="G150">
         <v>269.3370609356932</v>
@@ -3865,7 +3865,7 @@
         <v>2609760576.915093</v>
       </c>
       <c r="F151">
-        <v>-26807557.21697785</v>
+        <v>26807557.21697785</v>
       </c>
       <c r="G151">
         <v>5.522659147667259</v>
@@ -3888,7 +3888,7 @@
         <v>2701662462.370373</v>
       </c>
       <c r="F152">
-        <v>-22456878.06023574</v>
+        <v>22456878.06023574</v>
       </c>
       <c r="G152">
         <v>430.6616944641905</v>
@@ -3911,7 +3911,7 @@
         <v>2373912766.56643</v>
       </c>
       <c r="F153">
-        <v>-6287354.073957154</v>
+        <v>6287354.073957154</v>
       </c>
       <c r="G153">
         <v>40.46949130141842</v>
@@ -3934,7 +3934,7 @@
         <v>2288132164.547809</v>
       </c>
       <c r="F154">
-        <v>-51227219.09015395</v>
+        <v>51227219.09015395</v>
       </c>
       <c r="G154">
         <v>495.9563745355763</v>
@@ -3957,7 +3957,7 @@
         <v>2344624347.877722</v>
       </c>
       <c r="F155">
-        <v>-3006011.11654563</v>
+        <v>3006011.11654563</v>
       </c>
       <c r="G155">
         <v>191.0072361620598</v>
@@ -3980,7 +3980,7 @@
         <v>2324035744.369361</v>
       </c>
       <c r="F156">
-        <v>39089639.85088311</v>
+        <v>-39089639.85088311</v>
       </c>
       <c r="G156">
         <v>36.7033088949083</v>
@@ -4003,7 +4003,7 @@
         <v>1935730441.132565</v>
       </c>
       <c r="F157">
-        <v>-120891807.0093691</v>
+        <v>120891807.0093691</v>
       </c>
       <c r="G157">
         <v>208.5370214600775</v>
@@ -4026,7 +4026,7 @@
         <v>3128094910.877211</v>
       </c>
       <c r="F158">
-        <v>12752656.47561182</v>
+        <v>-12752656.47561182</v>
       </c>
       <c r="G158">
         <v>142.5940394123858</v>
@@ -4049,7 +4049,7 @@
         <v>2985467084.742025</v>
       </c>
       <c r="F159">
-        <v>7865713.081280822</v>
+        <v>-7865713.081280822</v>
       </c>
       <c r="G159">
         <v>321.5504153084832</v>
@@ -4072,7 +4072,7 @@
         <v>2539554703.956648</v>
       </c>
       <c r="F160">
-        <v>28550976.2097047</v>
+        <v>-28550976.2097047</v>
       </c>
       <c r="G160">
         <v>133.1104821214017</v>
@@ -4095,7 +4095,7 @@
         <v>2122137809.853559</v>
       </c>
       <c r="F161">
-        <v>-65936362.86466946</v>
+        <v>65936362.86466946</v>
       </c>
       <c r="G161">
         <v>313.5581417605769</v>
@@ -4118,7 +4118,7 @@
         <v>3267782809.83175</v>
       </c>
       <c r="F162">
-        <v>32685213.94314819</v>
+        <v>-32685213.94314819</v>
       </c>
       <c r="G162">
         <v>382.7298065708976</v>
@@ -4141,7 +4141,7 @@
         <v>2549208199.796457</v>
       </c>
       <c r="F163">
-        <v>-15129787.24873984</v>
+        <v>15129787.24873984</v>
       </c>
       <c r="G163">
         <v>116.4342485451196</v>
@@ -4164,7 +4164,7 @@
         <v>2910109884.384812</v>
       </c>
       <c r="F164">
-        <v>11321095.68117637</v>
+        <v>-11321095.68117637</v>
       </c>
       <c r="G164">
         <v>430.8414697035229</v>
@@ -4187,7 +4187,7 @@
         <v>3265067322.629371</v>
       </c>
       <c r="F165">
-        <v>-2226455.036940136</v>
+        <v>2226455.036940136</v>
       </c>
       <c r="G165">
         <v>377.4228902383945</v>
@@ -4210,7 +4210,7 @@
         <v>2365213727.85796</v>
       </c>
       <c r="F166">
-        <v>30673859.85569298</v>
+        <v>-30673859.85569298</v>
       </c>
       <c r="G166">
         <v>326.1821565130869</v>
@@ -4233,7 +4233,7 @@
         <v>2429909011.294053</v>
       </c>
       <c r="F167">
-        <v>-16523722.63063598</v>
+        <v>16523722.63063598</v>
       </c>
       <c r="G167">
         <v>405.6016304391342</v>
@@ -4256,7 +4256,7 @@
         <v>3024902844.993293</v>
       </c>
       <c r="F168">
-        <v>26526815.54057986</v>
+        <v>-26526815.54057986</v>
       </c>
       <c r="G168">
         <v>544.7055824357349</v>
@@ -4279,7 +4279,7 @@
         <v>2935604332.999224</v>
       </c>
       <c r="F169">
-        <v>-9043179.713305684</v>
+        <v>9043179.713305684</v>
       </c>
       <c r="G169">
         <v>70.21986776515132</v>
@@ -4302,7 +4302,7 @@
         <v>2969276017.595953</v>
       </c>
       <c r="F170">
-        <v>45951324.73962834</v>
+        <v>-45951324.73962834</v>
       </c>
       <c r="G170">
         <v>118.6938124995394</v>
@@ -4325,7 +4325,7 @@
         <v>2397325331.73465</v>
       </c>
       <c r="F171">
-        <v>-35583227.94198732</v>
+        <v>35583227.94198732</v>
       </c>
       <c r="G171">
         <v>89.6087900242761</v>
@@ -4348,7 +4348,7 @@
         <v>1090461313.019374</v>
       </c>
       <c r="F172">
-        <v>-83037663.30621134</v>
+        <v>83037663.30621134</v>
       </c>
       <c r="G172">
         <v>317.188266800946</v>
@@ -4371,7 +4371,7 @@
         <v>505954929.6191821</v>
       </c>
       <c r="F173">
-        <v>-315653138.2201879</v>
+        <v>315653138.2201879</v>
       </c>
       <c r="G173">
         <v>114.684419813436</v>
@@ -4394,7 +4394,7 @@
         <v>2634097295.423865</v>
       </c>
       <c r="F174">
-        <v>14186611.91552306</v>
+        <v>-14186611.91552306</v>
       </c>
       <c r="G174">
         <v>316.651054994061</v>
@@ -4417,7 +4417,7 @@
         <v>2153922306.858066</v>
       </c>
       <c r="F175">
-        <v>-104028839.900463</v>
+        <v>104028839.900463</v>
       </c>
       <c r="G175">
         <v>121.3139475424352</v>
@@ -4440,7 +4440,7 @@
         <v>1992678221.439851</v>
       </c>
       <c r="F176">
-        <v>-84275469.41572106</v>
+        <v>84275469.41572106</v>
       </c>
       <c r="G176">
         <v>-62.16544229493469</v>
@@ -4463,7 +4463,7 @@
         <v>997664084.8940914</v>
       </c>
       <c r="F177">
-        <v>331335589.3247173</v>
+        <v>-331335589.3247173</v>
       </c>
       <c r="G177">
         <v>-95.85160748423247</v>
@@ -4486,7 +4486,7 @@
         <v>2738149516.287169</v>
       </c>
       <c r="F178">
-        <v>-5315605.952762325</v>
+        <v>5315605.952762325</v>
       </c>
       <c r="G178">
         <v>150.1209848485497</v>
@@ -4509,7 +4509,7 @@
         <v>2265164718.023444</v>
       </c>
       <c r="F179">
-        <v>39205278.65236276</v>
+        <v>-39205278.65236276</v>
       </c>
       <c r="G179">
         <v>-158.6194640879232</v>
@@ -4532,7 +4532,7 @@
         <v>3196825565.453818</v>
       </c>
       <c r="F180">
-        <v>39561255.61846042</v>
+        <v>-39561255.61846042</v>
       </c>
       <c r="G180">
         <v>100.4256205295912</v>
@@ -4555,7 +4555,7 @@
         <v>1499806598.330992</v>
       </c>
       <c r="F181">
-        <v>27980409.52283004</v>
+        <v>-27980409.52283004</v>
       </c>
       <c r="G181">
         <v>54.53187711609101</v>
@@ -4578,7 +4578,7 @@
         <v>3471452045.405795</v>
       </c>
       <c r="F182">
-        <v>-28622477.40795692</v>
+        <v>28622477.40795692</v>
       </c>
       <c r="G182">
         <v>64.7249906789629</v>
@@ -4601,7 +4601,7 @@
         <v>2868653579.087183</v>
       </c>
       <c r="F183">
-        <v>9407379.650744831</v>
+        <v>-9407379.650744831</v>
       </c>
       <c r="G183">
         <v>134.4768316275478</v>
@@ -4624,7 +4624,7 @@
         <v>2012332774.739811</v>
       </c>
       <c r="F184">
-        <v>52585171.57564016</v>
+        <v>-52585171.57564016</v>
       </c>
       <c r="G184">
         <v>134.4369652716454</v>
@@ -4647,7 +4647,7 @@
         <v>2297603256.137409</v>
       </c>
       <c r="F185">
-        <v>55151778.96647949</v>
+        <v>-55151778.96647949</v>
       </c>
       <c r="G185">
         <v>83.61924462412458</v>
@@ -4670,7 +4670,7 @@
         <v>3115670104.780177</v>
       </c>
       <c r="F186">
-        <v>-20684258.06144327</v>
+        <v>20684258.06144327</v>
       </c>
       <c r="G186">
         <v>93.53874735469434</v>
@@ -4693,7 +4693,7 @@
         <v>2184124492.427251</v>
       </c>
       <c r="F187">
-        <v>59042938.8992428</v>
+        <v>-59042938.8992428</v>
       </c>
       <c r="G187">
         <v>34.6268981373526</v>
@@ -4716,7 +4716,7 @@
         <v>2313138605.45255</v>
       </c>
       <c r="F188">
-        <v>12747770.98337865</v>
+        <v>-12747770.98337865</v>
       </c>
       <c r="G188">
         <v>111.8581796353327</v>
@@ -4739,7 +4739,7 @@
         <v>2741667337.789729</v>
       </c>
       <c r="F189">
-        <v>33404815.53269046</v>
+        <v>-33404815.53269046</v>
       </c>
       <c r="G189">
         <v>-47.22208851763329</v>
@@ -4762,7 +4762,7 @@
         <v>1991439345.439217</v>
       </c>
       <c r="F190">
-        <v>128796335.2339712</v>
+        <v>-128796335.2339712</v>
       </c>
       <c r="G190">
         <v>141.7758727360583</v>
@@ -4785,7 +4785,7 @@
         <v>1418031621.297791</v>
       </c>
       <c r="F191">
-        <v>75556569.19388327</v>
+        <v>-75556569.19388327</v>
       </c>
       <c r="G191">
         <v>-32.44086179078059</v>
@@ -4808,7 +4808,7 @@
         <v>3644141551.465208</v>
       </c>
       <c r="F192">
-        <v>85997863.85278149</v>
+        <v>-85997863.85278149</v>
       </c>
       <c r="G192">
         <v>-67.56613940223765</v>

</xml_diff>